<commit_message>
Added total xp to XP spreadsheet
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\game\gameideas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\request\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>level</t>
   </si>
@@ -33,6 +33,12 @@
   </si>
   <si>
     <t>required XP</t>
+  </si>
+  <si>
+    <t>total xp</t>
+  </si>
+  <si>
+    <t>*didn't divide by 4</t>
   </si>
 </sst>
 </file>
@@ -3081,7 +3087,7 @@
   <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,142 +3095,204 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>400</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <f>B3+C2</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>600</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">B4+C3</f>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>800</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>900</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <f t="shared" ref="B4:B67" si="0">_xlfn.FLOOR.MATH(A7+500 * POWER(2, A7/6))</f>
+        <f t="shared" ref="B7:B67" si="1">_xlfn.FLOOR.MATH(A7+500 * POWER(2, A7/6))</f>
         <v>1006</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>3706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1129</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>4835</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1267</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>6102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1423</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>7525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1597</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>9122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1792</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10914</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2012</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>12926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2257</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>15183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2533</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>17716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2843</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>20559</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -3232,8 +3300,12 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3190</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>23749</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3241,8 +3313,12 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3580</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>27329</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3250,8 +3326,12 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4018</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>31347</v>
       </c>
       <c r="J19" t="s">
         <v>1</v>
@@ -3262,8 +3342,15 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4508</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>35855</v>
+      </c>
+      <c r="J20" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3271,8 +3358,12 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5059</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>40914</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3280,8 +3371,12 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5677</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>46591</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3289,8 +3384,12 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6371</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>52962</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3298,8 +3397,12 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7150</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>60112</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3307,8 +3410,12 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8024</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>68136</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3316,8 +3423,12 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9004</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>77140</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3325,8 +3436,12 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10105</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>87245</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3334,8 +3449,12 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11340</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>98585</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -3343,8 +3462,12 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12727</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>111312</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -3352,8 +3475,12 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>14283</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>125595</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -3361,8 +3488,12 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16030</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>141625</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
@@ -3370,1529 +3501,2209 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17990</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>159615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20190</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>179805</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22660</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>202465</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25432</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>227897</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28543</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>256440</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32036</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>288476</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>35955</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>324431</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40355</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>364786</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>45293</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>410079</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>50836</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>460915</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>57058</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>517973</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>64042</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>582015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>71880</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>653895</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>80678</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>734573</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>90554</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>825127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>101639</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>926766</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>114082</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>1040848</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>128048</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1168896</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>143724</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>1312620</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>161319</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>1473939</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>181070</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>1655009</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>203239</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>1858248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>228123</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>2086371</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>256054</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>2342425</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>287405</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>2629830</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>322595</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>2952425</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>362095</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>3314520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>406432</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>3720952</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>456199</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>4177151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>512060</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>4689211</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>574761</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>5263972</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>645141</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>5909113</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>724140</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>6633253</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>812813</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>7446066</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>912345</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>8358411</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1024066</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>9382477</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68">
-        <f t="shared" ref="B68:B131" si="1">_xlfn.FLOOR.MATH(A68+500 * POWER(2, A68/6))</f>
+        <f t="shared" ref="B68:B131" si="2">_xlfn.FLOOR.MATH(A68+500 * POWER(2, A68/6))</f>
         <v>1149468</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" ref="C68:C131" si="3">B68+C67</f>
+        <v>10531945</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1290227</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f t="shared" si="3"/>
+        <v>11822172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1448223</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f t="shared" si="3"/>
+        <v>13270395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1625568</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f t="shared" si="3"/>
+        <v>14895963</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1824631</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f t="shared" si="3"/>
+        <v>16720594</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
       <c r="B73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2048072</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f t="shared" si="3"/>
+        <v>18768666</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
       <c r="B74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2298875</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f t="shared" si="3"/>
+        <v>21067541</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
       <c r="B75">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2580392</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f t="shared" si="3"/>
+        <v>23647933</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
       <c r="B76">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2896384</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <f t="shared" si="3"/>
+        <v>26544317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
       <c r="B77">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3251073</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <f t="shared" si="3"/>
+        <v>29795390</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
       <c r="B78">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3649198</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f t="shared" si="3"/>
+        <v>33444588</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
       <c r="B79">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4096078</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <f t="shared" si="3"/>
+        <v>37540666</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4597683</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f t="shared" si="3"/>
+        <v>42138349</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5160716</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <f t="shared" si="3"/>
+        <v>47299065</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5792699</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <f t="shared" si="3"/>
+        <v>53091764</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6502076</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" si="3"/>
+        <v>59593840</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7298325</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f t="shared" si="3"/>
+        <v>66892165</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8192084</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" si="3"/>
+        <v>75084249</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9195294</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f t="shared" si="3"/>
+        <v>84279543</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10321359</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <f t="shared" si="3"/>
+        <v>94600902</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>11585324</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f t="shared" si="3"/>
+        <v>106186226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13004077</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <f t="shared" si="3"/>
+        <v>119190303</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14596573</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <f t="shared" si="3"/>
+        <v>133786876</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16384090</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <f t="shared" si="3"/>
+        <v>150170966</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18390509</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f t="shared" si="3"/>
+        <v>168561475</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20642638</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f t="shared" si="3"/>
+        <v>189204113</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>23170568</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f t="shared" si="3"/>
+        <v>212374681</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>26008072</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <f t="shared" si="3"/>
+        <v>238382753</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>29193064</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <f t="shared" si="3"/>
+        <v>267575817</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>32768096</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <f t="shared" si="3"/>
+        <v>300343913</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>36780933</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <f t="shared" si="3"/>
+        <v>337124846</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
       <c r="B99">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41285190</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <f t="shared" si="3"/>
+        <v>378410036</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46341049</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <f t="shared" si="3"/>
+        <v>424751085</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>52016057</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <f t="shared" si="3"/>
+        <v>476767142</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>58386039</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f t="shared" si="3"/>
+        <v>535153181</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65536102</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <f t="shared" si="3"/>
+        <v>600689283</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>73561775</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <f t="shared" si="3"/>
+        <v>674251058</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>82570289</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <f t="shared" si="3"/>
+        <v>756821347</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>92682005</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <f t="shared" si="3"/>
+        <v>849503352</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>104032021</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <f t="shared" si="3"/>
+        <v>953535373</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
       <c r="B108">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>116771983</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <f t="shared" si="3"/>
+        <v>1070307356</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
       <c r="B109">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>131072108</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <f t="shared" si="3"/>
+        <v>1201379464</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
       <c r="B110">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>147123454</v>
       </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <f t="shared" si="3"/>
+        <v>1348502918</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
       <c r="B111">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>165140481</v>
       </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <f t="shared" si="3"/>
+        <v>1513643399</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
       <c r="B112">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>185363911</v>
       </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <f t="shared" si="3"/>
+        <v>1699007310</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
       <c r="B113">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>208063942</v>
       </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <f t="shared" si="3"/>
+        <v>1907071252</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
       <c r="B114">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>233543866</v>
       </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <f t="shared" si="3"/>
+        <v>2140615118</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
       <c r="B115">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>262144114</v>
       </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <f t="shared" si="3"/>
+        <v>2402759232</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>294246806</v>
       </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <f t="shared" si="3"/>
+        <v>2697006038</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>330280859</v>
       </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <f t="shared" si="3"/>
+        <v>3027286897</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>370727717</v>
       </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <f t="shared" si="3"/>
+        <v>3398014614</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>416127779</v>
       </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <f t="shared" si="3"/>
+        <v>3814142393</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>467087626</v>
       </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <f t="shared" si="3"/>
+        <v>4281230019</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>524288120</v>
       </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <f t="shared" si="3"/>
+        <v>4805518139</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
       <c r="B122">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>588493503</v>
       </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <f t="shared" si="3"/>
+        <v>5394011642</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>660561609</v>
       </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <f t="shared" si="3"/>
+        <v>6054573251</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
       <c r="B124">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>741455323</v>
       </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <f t="shared" si="3"/>
+        <v>6796028574</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
       <c r="B125">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>832255446</v>
       </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <f t="shared" si="3"/>
+        <v>7628284020</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
       <c r="B126">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>934175139</v>
       </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <f t="shared" si="3"/>
+        <v>8562459159</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
       <c r="B127">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1048576126</v>
       </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <f t="shared" si="3"/>
+        <v>9611035285</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
       <c r="B128">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1176986891</v>
       </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <f t="shared" si="3"/>
+        <v>10788022176</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
       <c r="B129">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1321123102</v>
       </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <f t="shared" si="3"/>
+        <v>12109145278</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
       <c r="B130">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1482910529</v>
       </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <f t="shared" si="3"/>
+        <v>13592055807</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
       <c r="B131">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1664510775</v>
       </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <f t="shared" si="3"/>
+        <v>15256566582</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
       <c r="B132">
-        <f t="shared" ref="B132:B195" si="2">_xlfn.FLOOR.MATH(A132+500 * POWER(2, A132/6))</f>
+        <f t="shared" ref="B132:B195" si="4">_xlfn.FLOOR.MATH(A132+500 * POWER(2, A132/6))</f>
         <v>1868350159</v>
       </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <f t="shared" ref="C132:C195" si="5">B132+C131</f>
+        <v>17124916741</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
       <c r="B133">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2097152132</v>
       </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <f t="shared" si="5"/>
+        <v>19222068873</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
       <c r="B134">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2353973662</v>
       </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <f t="shared" si="5"/>
+        <v>21576042535</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
       <c r="B135">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2642246083</v>
       </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <f t="shared" si="5"/>
+        <v>24218288618</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
       <c r="B136">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2965820935</v>
       </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <f t="shared" si="5"/>
+        <v>27184109553</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
       <c r="B137">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3329021426</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <f t="shared" si="5"/>
+        <v>30513130979</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
       <c r="B138">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>3736700194</v>
       </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <f t="shared" si="5"/>
+        <v>34249831173</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
       <c r="B139">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4194304138</v>
       </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <f t="shared" si="5"/>
+        <v>38444135311</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
       <c r="B140">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4707947198</v>
       </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <f t="shared" si="5"/>
+        <v>43152082509</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
       <c r="B141">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5284492039</v>
       </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C141">
+        <f t="shared" si="5"/>
+        <v>48436574548</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
       <c r="B142">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5931641742</v>
       </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C142">
+        <f t="shared" si="5"/>
+        <v>54368216290</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
       <c r="B143">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6658042723</v>
       </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C143">
+        <f t="shared" si="5"/>
+        <v>61026259013</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
       <c r="B144">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7473400257</v>
       </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <f t="shared" si="5"/>
+        <v>68499659270</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
       <c r="B145">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8388608144</v>
       </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C145">
+        <f t="shared" si="5"/>
+        <v>76888267414</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
       <c r="B146">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>9415894263</v>
       </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C146">
+        <f t="shared" si="5"/>
+        <v>86304161677</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
       <c r="B147">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>10568983944</v>
       </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <f t="shared" si="5"/>
+        <v>96873145621</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
       <c r="B148">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>11863283350</v>
       </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <f t="shared" si="5"/>
+        <v>108736428971</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
       <c r="B149">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>13316085311</v>
       </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <f t="shared" si="5"/>
+        <v>122052514282</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
       <c r="B150">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>14946800377</v>
       </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <f t="shared" si="5"/>
+        <v>136999314659</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
       <c r="B151">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>16777216150</v>
       </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <f t="shared" si="5"/>
+        <v>153776530809</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
       <c r="B152">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18831788387</v>
       </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <f t="shared" si="5"/>
+        <v>172608319196</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
       <c r="B153">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21137967749</v>
       </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <f t="shared" si="5"/>
+        <v>193746286945</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
       <c r="B154">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>23726566559</v>
       </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C154">
+        <f t="shared" si="5"/>
+        <v>217472853504</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
       <c r="B155">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26632170481</v>
       </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C155">
+        <f t="shared" si="5"/>
+        <v>244105023985</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
       <c r="B156">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29893600611</v>
       </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C156">
+        <f t="shared" si="5"/>
+        <v>273998624596</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33554432156</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C157">
+        <f t="shared" si="5"/>
+        <v>307553056752</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
       <c r="B158">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37663576629</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C158">
+        <f t="shared" si="5"/>
+        <v>345216633381</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
       <c r="B159">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42275935352</v>
       </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C159">
+        <f t="shared" si="5"/>
+        <v>387492568733</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
       <c r="B160">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47453132971</v>
       </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C160">
+        <f t="shared" si="5"/>
+        <v>434945701704</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>53264340814</v>
       </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C161">
+        <f t="shared" si="5"/>
+        <v>488210042518</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
       <c r="B162">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>59787201074</v>
       </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C162">
+        <f t="shared" si="5"/>
+        <v>547997243592</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>67108864162</v>
       </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C163">
+        <f t="shared" si="5"/>
+        <v>615106107754</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>75327153108</v>
       </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C164">
+        <f t="shared" si="5"/>
+        <v>690433260862</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>84551870552</v>
       </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C165">
+        <f t="shared" si="5"/>
+        <v>774985131414</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>94906265789</v>
       </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C166">
+        <f t="shared" si="5"/>
+        <v>869891397203</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
       <c r="B167">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>106528681475</v>
       </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C167">
+        <f t="shared" si="5"/>
+        <v>976420078678</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
       <c r="B168">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>119574401993</v>
       </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C168">
+        <f t="shared" si="5"/>
+        <v>1095994480671</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
       <c r="B169">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>134217728168</v>
       </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C169">
+        <f t="shared" si="5"/>
+        <v>1230212208839</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
       <c r="B170">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>150654306059</v>
       </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C170">
+        <f t="shared" si="5"/>
+        <v>1380866514898</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
       <c r="B171">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>169103740946</v>
       </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C171">
+        <f t="shared" si="5"/>
+        <v>1549970255844</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
       <c r="B172">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>189812531419</v>
       </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C172">
+        <f t="shared" si="5"/>
+        <v>1739782787263</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
       <c r="B173">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>213057362791</v>
       </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C173">
+        <f t="shared" si="5"/>
+        <v>1952840150054</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
       <c r="B174">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>239148803826</v>
       </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C174">
+        <f t="shared" si="5"/>
+        <v>2191988953880</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
       <c r="B175">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>268435456174</v>
       </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C175">
+        <f t="shared" si="5"/>
+        <v>2460424410054</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
       <c r="B176">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>301308611955</v>
       </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C176">
+        <f t="shared" si="5"/>
+        <v>2761733022009</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
       <c r="B177">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>338207481728</v>
       </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C177">
+        <f t="shared" si="5"/>
+        <v>3099940503737</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
       <c r="B178">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>379625062674</v>
       </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C178">
+        <f t="shared" si="5"/>
+        <v>3479565566411</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
       <c r="B179">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>426114725417</v>
       </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C179">
+        <f t="shared" si="5"/>
+        <v>3905680291828</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
       <c r="B180">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>478297607486</v>
       </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C180">
+        <f t="shared" si="5"/>
+        <v>4383977899314</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
       <c r="B181">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>536870912180</v>
       </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C181">
+        <f t="shared" si="5"/>
+        <v>4920848811494</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
       <c r="B182">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>602617223742</v>
       </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C182">
+        <f t="shared" si="5"/>
+        <v>5523466035236</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
       <c r="B183">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>676414963287</v>
       </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C183">
+        <f t="shared" si="5"/>
+        <v>6199880998523</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
       <c r="B184">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>759250125177</v>
       </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C184">
+        <f t="shared" si="5"/>
+        <v>6959131123700</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
       <c r="B185">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>852229450663</v>
       </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C185">
+        <f t="shared" si="5"/>
+        <v>7811360574363</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
       <c r="B186">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>956595214800</v>
       </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C186">
+        <f t="shared" si="5"/>
+        <v>8767955789163</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
       <c r="B187">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1073741824186</v>
       </c>
-    </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C187">
+        <f t="shared" si="5"/>
+        <v>9841697613349</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
       <c r="B188">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1205234447309</v>
       </c>
-    </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C188">
+        <f t="shared" si="5"/>
+        <v>11046932060658</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
       <c r="B189">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1352829926398</v>
       </c>
-    </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C189">
+        <f t="shared" si="5"/>
+        <v>12399761987056</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
       <c r="B190">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1518500250177</v>
       </c>
-    </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C190">
+        <f t="shared" si="5"/>
+        <v>13918262237233</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
       <c r="B191">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1704458901149</v>
       </c>
-    </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C191">
+        <f t="shared" si="5"/>
+        <v>15622721138382</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
       <c r="B192">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1913190429421</v>
       </c>
-    </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C192">
+        <f t="shared" si="5"/>
+        <v>17535911567803</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
       <c r="B193">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2147483648192</v>
       </c>
-    </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C193">
+        <f t="shared" si="5"/>
+        <v>19683395215995</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
       <c r="B194">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2410468894437</v>
       </c>
-    </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C194">
+        <f t="shared" si="5"/>
+        <v>22093864110432</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
       <c r="B195">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>2705659852614</v>
       </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C195">
+        <f t="shared" si="5"/>
+        <v>24799523963046</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
       <c r="B196">
-        <f t="shared" ref="B196:B201" si="3">_xlfn.FLOOR.MATH(A196+500 * POWER(2, A196/6))</f>
+        <f t="shared" ref="B196:B201" si="6">_xlfn.FLOOR.MATH(A196+500 * POWER(2, A196/6))</f>
         <v>3037000500171</v>
       </c>
-    </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C196">
+        <f t="shared" ref="C196:C201" si="7">B196+C195</f>
+        <v>27836524463217</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
       <c r="B197">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3408917802115</v>
       </c>
-    </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C197">
+        <f t="shared" si="7"/>
+        <v>31245442265332</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
       <c r="B198">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3826380858658</v>
       </c>
-    </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C198">
+        <f t="shared" si="7"/>
+        <v>35071823123990</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
       <c r="B199">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4294967296198</v>
       </c>
-    </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C199">
+        <f t="shared" si="7"/>
+        <v>39366790420188</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
       <c r="B200">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4820937788688</v>
       </c>
-    </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C200">
+        <f t="shared" si="7"/>
+        <v>44187728208876</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
       <c r="B201">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>5411319705040</v>
+      </c>
+      <c r="C201">
+        <f t="shared" si="7"/>
+        <v>49599047913916</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added attack types and damage type tables and pages on data seeder
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
+    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>level</t>
   </si>
@@ -39,6 +40,60 @@
   </si>
   <si>
     <t>*didn't divide by 4</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Damage Type</t>
+  </si>
+  <si>
+    <t>Base Damage</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Base Item Chance</t>
+  </si>
+  <si>
+    <t>Base Gold Chance</t>
+  </si>
+  <si>
+    <t>Base Gold Amount</t>
+  </si>
+  <si>
+    <t>Rarity</t>
+  </si>
+  <si>
+    <t>rarity will be the chance in which an enemy is generated</t>
+  </si>
+  <si>
+    <t>base item chance is the base amount in which enemy will drop an item</t>
+  </si>
+  <si>
+    <t>base gold amount is the base amount of gold which an enemy will drop</t>
+  </si>
+  <si>
+    <t>base gold chance is the base amount in which enemy will drop gold</t>
+  </si>
+  <si>
+    <t>experience is the amount in which a single instance of this enemy will reward</t>
+  </si>
+  <si>
+    <t>base damage is the base damage amount (before multipliers) that his enemy will inflict</t>
+  </si>
+  <si>
+    <t>melee, projectile, elemental-fire, elemental-ice, elemental-electric</t>
+  </si>
+  <si>
+    <t>enemy type is used to determine which enemy is to be rendered</t>
   </si>
 </sst>
 </file>
@@ -74,8 +129,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3086,7 +3144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -5710,4 +5768,81 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="10" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added some table notes to spreadsheet
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
     <sheet name="Enemies" sheetId="2" r:id="rId2"/>
+    <sheet name="Damage Types" sheetId="3" r:id="rId3"/>
+    <sheet name="Attack Type" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>level</t>
   </si>
@@ -48,12 +50,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Damage Type</t>
-  </si>
-  <si>
     <t>Base Damage</t>
   </si>
   <si>
@@ -67,9 +63,6 @@
   </si>
   <si>
     <t>Base Gold Amount</t>
-  </si>
-  <si>
-    <t>Rarity</t>
   </si>
   <si>
     <t>rarity will be the chance in which an enemy is generated</t>
@@ -93,7 +86,40 @@
     <t>melee, projectile, elemental-fire, elemental-ice, elemental-electric</t>
   </si>
   <si>
-    <t>enemy type is used to determine which enemy is to be rendered</t>
+    <t>Rarity (0-100)</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Sprite</t>
+  </si>
+  <si>
+    <t>determines which sprite is rendered for an enemy</t>
+  </si>
+  <si>
+    <t>Melee</t>
+  </si>
+  <si>
+    <t>Projectile</t>
+  </si>
+  <si>
+    <t>Elemental-Fire</t>
+  </si>
+  <si>
+    <t>Elemental-Ice</t>
+  </si>
+  <si>
+    <t>Elemental-Electric</t>
+  </si>
+  <si>
+    <t>Attack_Type_Id</t>
+  </si>
+  <si>
+    <t>Attack_Type_Name</t>
+  </si>
+  <si>
+    <t>damage_type_id</t>
   </si>
 </sst>
 </file>
@@ -5774,8 +5800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5791,28 +5817,28 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.25">
@@ -5820,29 +5846,160 @@
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated numbers in spreadsheet, added monster to page
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
-    <sheet name="Enemies" sheetId="2" r:id="rId2"/>
+    <sheet name="Monsters" sheetId="2" r:id="rId2"/>
     <sheet name="d2 mean mlvl" sheetId="6" r:id="rId3"/>
     <sheet name="Damage Types" sheetId="3" r:id="rId4"/>
     <sheet name="Attack Type" sheetId="4" r:id="rId5"/>
@@ -190,12 +190,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -210,12 +216,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4673,13 +4681,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4692,10 +4701,10 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -4709,7 +4718,7 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>0</v>
       </c>
     </row>
@@ -4724,10 +4733,10 @@
         <f>B3+C2</f>
         <v>500</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>500</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <f>D3+E2</f>
         <v>500</v>
       </c>
@@ -4743,10 +4752,10 @@
         <f t="shared" ref="C4:C67" si="0">B4+C3</f>
         <v>1500</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>1500</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <f t="shared" ref="E4:E67" si="1">D4+E3</f>
         <v>2000</v>
       </c>
@@ -4762,10 +4771,10 @@
         <f t="shared" si="0"/>
         <v>3750</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>3750</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <f t="shared" si="1"/>
         <v>5750</v>
       </c>
@@ -4781,10 +4790,10 @@
         <f t="shared" si="0"/>
         <v>7875</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>7875</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <f t="shared" si="1"/>
         <v>13625</v>
       </c>
@@ -4800,10 +4809,10 @@
         <f t="shared" si="0"/>
         <v>14175</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>14175</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <f t="shared" si="1"/>
         <v>27800</v>
       </c>
@@ -4820,10 +4829,10 @@
         <f t="shared" si="0"/>
         <v>15304</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>22680</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <f t="shared" si="1"/>
         <v>50480</v>
       </c>
@@ -4840,10 +4849,10 @@
         <f t="shared" si="0"/>
         <v>16571</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>32886</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="3">
         <f t="shared" si="1"/>
         <v>83366</v>
       </c>
@@ -4860,10 +4869,10 @@
         <f t="shared" si="0"/>
         <v>17994</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>44396</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <f t="shared" si="1"/>
         <v>127762</v>
       </c>
@@ -4880,10 +4889,10 @@
         <f t="shared" si="0"/>
         <v>19591</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>57715</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="3">
         <f t="shared" si="1"/>
         <v>185477</v>
       </c>
@@ -4900,10 +4909,10 @@
         <f t="shared" si="0"/>
         <v>21383</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>72144</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="3">
         <f t="shared" si="1"/>
         <v>257621</v>
       </c>
@@ -4920,11 +4929,11 @@
         <f t="shared" si="0"/>
         <v>23395</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <f>D12*1.25</f>
         <v>90180</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="3">
         <f t="shared" si="1"/>
         <v>347801</v>
       </c>
@@ -4941,11 +4950,11 @@
         <f t="shared" si="0"/>
         <v>25652</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="3">
         <f>D13*1.25</f>
         <v>112725</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="3">
         <f t="shared" si="1"/>
         <v>460526</v>
       </c>
@@ -4962,11 +4971,11 @@
         <f t="shared" si="0"/>
         <v>28185</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="3">
         <f t="shared" ref="D15:D28" si="3">D14*1.25</f>
         <v>140906.25</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="3">
         <f t="shared" si="1"/>
         <v>601432.25</v>
       </c>
@@ -4983,11 +4992,11 @@
         <f t="shared" si="0"/>
         <v>31028</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <f t="shared" si="3"/>
         <v>176132.8125</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="3">
         <f t="shared" si="1"/>
         <v>777565.0625</v>
       </c>
@@ -5004,11 +5013,11 @@
         <f t="shared" si="0"/>
         <v>34218</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="3">
         <f t="shared" si="3"/>
         <v>220166.015625</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="3">
         <f t="shared" si="1"/>
         <v>997731.078125</v>
       </c>
@@ -5025,11 +5034,11 @@
         <f t="shared" si="0"/>
         <v>37798</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <f t="shared" si="3"/>
         <v>275207.51953125</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="3">
         <f t="shared" si="1"/>
         <v>1272938.59765625</v>
       </c>
@@ -5046,11 +5055,11 @@
         <f t="shared" si="0"/>
         <v>41816</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="3">
         <f t="shared" si="3"/>
         <v>344009.3994140625</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="3">
         <f t="shared" si="1"/>
         <v>1616947.9970703125</v>
       </c>
@@ -5070,11 +5079,11 @@
         <f t="shared" si="0"/>
         <v>46324</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="3">
         <f t="shared" si="3"/>
         <v>430011.74926757813</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="3">
         <f t="shared" si="1"/>
         <v>2046959.7463378906</v>
       </c>
@@ -5097,11 +5106,11 @@
         <f t="shared" si="0"/>
         <v>51383</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="3">
         <f t="shared" si="3"/>
         <v>537514.68658447266</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="3">
         <f t="shared" si="1"/>
         <v>2584474.4329223633</v>
       </c>
@@ -5124,11 +5133,11 @@
         <f t="shared" si="0"/>
         <v>57060</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="3">
         <f t="shared" si="3"/>
         <v>671893.35823059082</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="3">
         <f t="shared" si="1"/>
         <v>3256367.7911529541</v>
       </c>
@@ -5148,11 +5157,11 @@
         <f t="shared" si="0"/>
         <v>63431</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <f t="shared" si="3"/>
         <v>839866.69778823853</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="3">
         <f t="shared" si="1"/>
         <v>4096234.4889411926</v>
       </c>
@@ -5169,11 +5178,11 @@
         <f t="shared" si="0"/>
         <v>70581</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="3">
         <f t="shared" si="3"/>
         <v>1049833.3722352982</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="3">
         <f t="shared" si="1"/>
         <v>5146067.8611764908</v>
       </c>
@@ -5190,11 +5199,11 @@
         <f t="shared" si="0"/>
         <v>78605</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="3">
         <f t="shared" si="3"/>
         <v>1312291.7152941227</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="3">
         <f t="shared" si="1"/>
         <v>6458359.5764706135</v>
       </c>
@@ -5211,11 +5220,11 @@
         <f t="shared" si="0"/>
         <v>87609</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="3">
         <f t="shared" si="3"/>
         <v>1640364.6441176534</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="3">
         <f t="shared" si="1"/>
         <v>8098724.2205882668</v>
       </c>
@@ -5232,11 +5241,11 @@
         <f t="shared" si="0"/>
         <v>97714</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="3">
         <f t="shared" si="3"/>
         <v>2050455.8051470667</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="3">
         <f t="shared" si="1"/>
         <v>10149180.025735334</v>
       </c>
@@ -5253,11 +5262,11 @@
         <f t="shared" si="0"/>
         <v>109054</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <f t="shared" si="3"/>
         <v>2563069.7564338334</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="3">
         <f t="shared" si="1"/>
         <v>12712249.782169167</v>
       </c>
@@ -5274,11 +5283,11 @@
         <f t="shared" si="0"/>
         <v>121781</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="3">
         <f>D28*1.25</f>
         <v>3203837.1955422917</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="3">
         <f t="shared" si="1"/>
         <v>15916086.977711458</v>
       </c>
@@ -5295,11 +5304,11 @@
         <f t="shared" si="0"/>
         <v>136064</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="3">
         <f t="shared" ref="D30" si="4">D29*1.25</f>
         <v>4004796.4944278644</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="3">
         <f t="shared" si="1"/>
         <v>19920883.472139321</v>
       </c>
@@ -5316,11 +5325,11 @@
         <f t="shared" si="0"/>
         <v>152094</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="3">
         <f>D30*1.158</f>
         <v>4637554.3405474667</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="3">
         <f t="shared" si="1"/>
         <v>24558437.812686786</v>
       </c>
@@ -5337,11 +5346,11 @@
         <f t="shared" si="0"/>
         <v>170084</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="3">
         <f t="shared" ref="D32:D95" si="5">D31*1.158</f>
         <v>5370287.9263539659</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="3">
         <f t="shared" si="1"/>
         <v>29928725.739040751</v>
       </c>
@@ -5358,11 +5367,11 @@
         <f t="shared" si="0"/>
         <v>190274</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="3">
         <f t="shared" si="5"/>
         <v>6218793.4187178919</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="3">
         <f t="shared" si="1"/>
         <v>36147519.157758646</v>
       </c>
@@ -5379,11 +5388,11 @@
         <f t="shared" si="0"/>
         <v>212934</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <f t="shared" si="5"/>
         <v>7201362.7788753184</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="3">
         <f t="shared" si="1"/>
         <v>43348881.936633967</v>
       </c>
@@ -5400,11 +5409,11 @@
         <f t="shared" si="0"/>
         <v>238366</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="3">
         <f t="shared" si="5"/>
         <v>8339178.0979376184</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="3">
         <f t="shared" si="1"/>
         <v>51688060.034571588</v>
       </c>
@@ -5421,11 +5430,11 @@
         <f t="shared" si="0"/>
         <v>266909</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="3">
         <f t="shared" si="5"/>
         <v>9656768.2374117617</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="3">
         <f t="shared" si="1"/>
         <v>61344828.271983348</v>
       </c>
@@ -5442,11 +5451,11 @@
         <f t="shared" si="0"/>
         <v>298945</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="3">
         <f t="shared" si="5"/>
         <v>11182537.618922818</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="3">
         <f t="shared" si="1"/>
         <v>72527365.89090617</v>
       </c>
@@ -5463,11 +5472,11 @@
         <f t="shared" si="0"/>
         <v>334900</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="3">
         <f t="shared" si="5"/>
         <v>12949378.562712623</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="3">
         <f t="shared" si="1"/>
         <v>85476744.453618795</v>
       </c>
@@ -5484,11 +5493,11 @@
         <f t="shared" si="0"/>
         <v>375255</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="3">
         <f t="shared" si="5"/>
         <v>14995380.375621216</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="3">
         <f t="shared" si="1"/>
         <v>100472124.82924001</v>
       </c>
@@ -5505,11 +5514,11 @@
         <f t="shared" si="0"/>
         <v>420548</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="3">
         <f t="shared" si="5"/>
         <v>17364650.474969368</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="3">
         <f t="shared" si="1"/>
         <v>117836775.30420938</v>
       </c>
@@ -5526,11 +5535,11 @@
         <f t="shared" si="0"/>
         <v>471384</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="3">
         <f t="shared" si="5"/>
         <v>20108265.250014529</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="3">
         <f t="shared" si="1"/>
         <v>137945040.5542239</v>
       </c>
@@ -5547,11 +5556,11 @@
         <f t="shared" si="0"/>
         <v>528442</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="3">
         <f t="shared" si="5"/>
         <v>23285371.159516823</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="3">
         <f t="shared" si="1"/>
         <v>161230411.71374071</v>
       </c>
@@ -5568,11 +5577,11 @@
         <f t="shared" si="0"/>
         <v>592484</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="3">
         <f t="shared" si="5"/>
         <v>26964459.80272048</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="3">
         <f t="shared" si="1"/>
         <v>188194871.51646119</v>
       </c>
@@ -5589,11 +5598,11 @@
         <f t="shared" si="0"/>
         <v>664364</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="3">
         <f t="shared" si="5"/>
         <v>31224844.451550312</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="3">
         <f t="shared" si="1"/>
         <v>219419715.9680115</v>
       </c>
@@ -5610,11 +5619,11 @@
         <f t="shared" si="0"/>
         <v>745042</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="3">
         <f t="shared" si="5"/>
         <v>36158369.87489526</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="3">
         <f t="shared" si="1"/>
         <v>255578085.84290677</v>
       </c>
@@ -5631,11 +5640,11 @@
         <f t="shared" si="0"/>
         <v>835596</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="3">
         <f t="shared" si="5"/>
         <v>41871392.315128706</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="3">
         <f t="shared" si="1"/>
         <v>297449478.15803546</v>
       </c>
@@ -5652,11 +5661,11 @@
         <f t="shared" si="0"/>
         <v>937235</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="3">
         <f t="shared" si="5"/>
         <v>48487072.300919041</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="3">
         <f t="shared" si="1"/>
         <v>345936550.45895451</v>
       </c>
@@ -5673,11 +5682,11 @@
         <f t="shared" si="0"/>
         <v>1051317</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="3">
         <f t="shared" si="5"/>
         <v>56148029.724464245</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="3">
         <f t="shared" si="1"/>
         <v>402084580.18341875</v>
       </c>
@@ -5694,11 +5703,11 @@
         <f t="shared" si="0"/>
         <v>1179365</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <f t="shared" si="5"/>
         <v>65019418.420929588</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="3">
         <f t="shared" si="1"/>
         <v>467103998.60434836</v>
       </c>
@@ -5715,11 +5724,11 @@
         <f t="shared" si="0"/>
         <v>1323089</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="3">
         <f t="shared" si="5"/>
         <v>75292486.531436458</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="3">
         <f t="shared" si="1"/>
         <v>542396485.13578486</v>
       </c>
@@ -5736,11 +5745,11 @@
         <f t="shared" si="0"/>
         <v>1484408</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="3">
         <f t="shared" si="5"/>
         <v>87188699.403403416</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="3">
         <f t="shared" si="1"/>
         <v>629585184.53918827</v>
       </c>
@@ -5757,11 +5766,11 @@
         <f t="shared" si="0"/>
         <v>1665478</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="3">
         <f t="shared" si="5"/>
         <v>100964513.90914115</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="3">
         <f t="shared" si="1"/>
         <v>730549698.44832945</v>
       </c>
@@ -5778,11 +5787,11 @@
         <f t="shared" si="0"/>
         <v>1868717</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="3">
         <f t="shared" si="5"/>
         <v>116916907.10678545</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="3">
         <f t="shared" si="1"/>
         <v>847466605.55511487</v>
       </c>
@@ -5799,11 +5808,11 @@
         <f t="shared" si="0"/>
         <v>2096840</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="3">
         <f t="shared" si="5"/>
         <v>135389778.42965755</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="3">
         <f t="shared" si="1"/>
         <v>982856383.98477244</v>
       </c>
@@ -5820,11 +5829,11 @@
         <f t="shared" si="0"/>
         <v>2352894</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="3">
         <f t="shared" si="5"/>
         <v>156781363.42154342</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="3">
         <f t="shared" si="1"/>
         <v>1139637747.4063158</v>
       </c>
@@ -5841,11 +5850,11 @@
         <f t="shared" si="0"/>
         <v>2640299</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="3">
         <f t="shared" si="5"/>
         <v>181552818.84214726</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="3">
         <f t="shared" si="1"/>
         <v>1321190566.2484632</v>
       </c>
@@ -5862,11 +5871,11 @@
         <f t="shared" si="0"/>
         <v>2962894</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="3">
         <f t="shared" si="5"/>
         <v>210238164.21920651</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="3">
         <f t="shared" si="1"/>
         <v>1531428730.4676697</v>
       </c>
@@ -5883,11 +5892,11 @@
         <f t="shared" si="0"/>
         <v>3324989</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="3">
         <f t="shared" si="5"/>
         <v>243455794.16584113</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="3">
         <f t="shared" si="1"/>
         <v>1774884524.6335108</v>
       </c>
@@ -5904,11 +5913,11 @@
         <f t="shared" si="0"/>
         <v>3731421</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="3">
         <f t="shared" si="5"/>
         <v>281921809.64404398</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="3">
         <f t="shared" si="1"/>
         <v>2056806334.2775548</v>
       </c>
@@ -5925,11 +5934,11 @@
         <f t="shared" si="0"/>
         <v>4187620</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="3">
         <f t="shared" si="5"/>
         <v>326465455.56780291</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="3">
         <f t="shared" si="1"/>
         <v>2383271789.8453579</v>
       </c>
@@ -5946,11 +5955,11 @@
         <f t="shared" si="0"/>
         <v>4699680</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="3">
         <f t="shared" si="5"/>
         <v>378046997.54751575</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="3">
         <f t="shared" si="1"/>
         <v>2761318787.3928738</v>
       </c>
@@ -5967,11 +5976,11 @@
         <f t="shared" si="0"/>
         <v>5274441</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="3">
         <f t="shared" si="5"/>
         <v>437778423.16002321</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="3">
         <f t="shared" si="1"/>
         <v>3199097210.552897</v>
       </c>
@@ -5988,11 +5997,11 @@
         <f t="shared" si="0"/>
         <v>5919582</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="3">
         <f t="shared" si="5"/>
         <v>506947414.01930684</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="3">
         <f t="shared" si="1"/>
         <v>3706044624.5722036</v>
       </c>
@@ -6009,11 +6018,11 @@
         <f t="shared" si="0"/>
         <v>6643722</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="3">
         <f t="shared" si="5"/>
         <v>587045105.43435729</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="3">
         <f t="shared" si="1"/>
         <v>4293089730.0065608</v>
       </c>
@@ -6030,11 +6039,11 @@
         <f t="shared" si="0"/>
         <v>7456535</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="3">
         <f t="shared" si="5"/>
         <v>679798232.09298563</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="3">
         <f t="shared" si="1"/>
         <v>4972887962.0995464</v>
       </c>
@@ -6051,11 +6060,11 @@
         <f t="shared" si="0"/>
         <v>8368880</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="3">
         <f t="shared" si="5"/>
         <v>787206352.76367736</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="3">
         <f t="shared" si="1"/>
         <v>5760094314.863224</v>
       </c>
@@ -6072,11 +6081,11 @@
         <f t="shared" si="0"/>
         <v>9392946</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="3">
         <f t="shared" si="5"/>
         <v>911584956.50033832</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="3">
         <f t="shared" si="1"/>
         <v>6671679271.3635626</v>
       </c>
@@ -6093,11 +6102,11 @@
         <f t="shared" ref="C68:C131" si="7">B68+C67</f>
         <v>10542414</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="3">
         <f t="shared" si="5"/>
         <v>1055615379.6273917</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="3">
         <f t="shared" ref="E68:E131" si="8">D68+E67</f>
         <v>7727294650.9909544</v>
       </c>
@@ -6114,11 +6123,11 @@
         <f t="shared" si="7"/>
         <v>11832641</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="3">
         <f t="shared" si="5"/>
         <v>1222402609.6085196</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="3">
         <f t="shared" si="8"/>
         <v>8949697260.599474</v>
       </c>
@@ -6135,11 +6144,11 @@
         <f t="shared" si="7"/>
         <v>13280864</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="3">
         <f t="shared" si="5"/>
         <v>1415542221.9266655</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="3">
         <f t="shared" si="8"/>
         <v>10365239482.52614</v>
       </c>
@@ -6156,11 +6165,11 @@
         <f t="shared" si="7"/>
         <v>14906432</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="3">
         <f t="shared" si="5"/>
         <v>1639197892.9910786</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="3">
         <f t="shared" si="8"/>
         <v>12004437375.51722</v>
       </c>
@@ -6177,11 +6186,11 @@
         <f t="shared" si="7"/>
         <v>16731063</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="3">
         <f t="shared" si="5"/>
         <v>1898191160.0836689</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="3">
         <f t="shared" si="8"/>
         <v>13902628535.600889</v>
       </c>
@@ -6198,11 +6207,11 @@
         <f t="shared" si="7"/>
         <v>18779135</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="3">
         <f t="shared" si="5"/>
         <v>2198105363.3768883</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="3">
         <f t="shared" si="8"/>
         <v>16100733898.977777</v>
       </c>
@@ -6219,11 +6228,11 @@
         <f t="shared" si="7"/>
         <v>21078010</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="3">
         <f t="shared" si="5"/>
         <v>2545406010.7904363</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="3">
         <f t="shared" si="8"/>
         <v>18646139909.768215</v>
       </c>
@@ -6240,11 +6249,11 @@
         <f t="shared" si="7"/>
         <v>23658402</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="3">
         <f t="shared" si="5"/>
         <v>2947580160.4953251</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="3">
         <f t="shared" si="8"/>
         <v>21593720070.263542</v>
       </c>
@@ -6261,11 +6270,11 @@
         <f t="shared" si="7"/>
         <v>26554786</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="3">
         <f t="shared" si="5"/>
         <v>3413297825.8535862</v>
       </c>
-      <c r="E76">
+      <c r="E76" s="3">
         <f t="shared" si="8"/>
         <v>25007017896.117126</v>
       </c>
@@ -6282,11 +6291,11 @@
         <f t="shared" si="7"/>
         <v>29805859</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="3">
         <f t="shared" si="5"/>
         <v>3952598882.3384523</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="3">
         <f t="shared" si="8"/>
         <v>28959616778.455578</v>
       </c>
@@ -6303,11 +6312,11 @@
         <f t="shared" si="7"/>
         <v>33455057</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="3">
         <f t="shared" si="5"/>
         <v>4577109505.7479277</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="3">
         <f t="shared" si="8"/>
         <v>33536726284.203506</v>
       </c>
@@ -6324,11 +6333,11 @@
         <f t="shared" si="7"/>
         <v>37551135</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="3">
         <f t="shared" si="5"/>
         <v>5300292807.6561003</v>
       </c>
-      <c r="E79">
+      <c r="E79" s="3">
         <f t="shared" si="8"/>
         <v>38837019091.859604</v>
       </c>
@@ -6345,11 +6354,11 @@
         <f t="shared" si="7"/>
         <v>42148818</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="3">
         <f t="shared" si="5"/>
         <v>6137739071.2657633</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="3">
         <f t="shared" si="8"/>
         <v>44974758163.125366</v>
       </c>
@@ -6366,11 +6375,11 @@
         <f t="shared" si="7"/>
         <v>47309534</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="3">
         <f t="shared" si="5"/>
         <v>7107501844.525753</v>
       </c>
-      <c r="E81">
+      <c r="E81" s="3">
         <f t="shared" si="8"/>
         <v>52082260007.651123</v>
       </c>
@@ -6387,11 +6396,11 @@
         <f t="shared" si="7"/>
         <v>53102233</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="3">
         <f t="shared" si="5"/>
         <v>8230487135.9608212</v>
       </c>
-      <c r="E82">
+      <c r="E82" s="3">
         <f t="shared" si="8"/>
         <v>60312747143.611946</v>
       </c>
@@ -6408,11 +6417,11 @@
         <f t="shared" si="7"/>
         <v>59604309</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="3">
         <f t="shared" si="5"/>
         <v>9530904103.4426308</v>
       </c>
-      <c r="E83">
+      <c r="E83" s="3">
         <f t="shared" si="8"/>
         <v>69843651247.054581</v>
       </c>
@@ -6429,11 +6438,11 @@
         <f t="shared" si="7"/>
         <v>66902634</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="3">
         <f t="shared" si="5"/>
         <v>11036786951.786566</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="3">
         <f t="shared" si="8"/>
         <v>80880438198.841141</v>
       </c>
@@ -6450,11 +6459,11 @@
         <f t="shared" si="7"/>
         <v>75094718</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="3">
         <f t="shared" si="5"/>
         <v>12780599290.168842</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="3">
         <f t="shared" si="8"/>
         <v>93661037489.009979</v>
       </c>
@@ -6471,11 +6480,11 @@
         <f t="shared" si="7"/>
         <v>84290012</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="3">
         <f t="shared" si="5"/>
         <v>14799933978.015518</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="3">
         <f t="shared" si="8"/>
         <v>108460971467.0255</v>
       </c>
@@ -6492,11 +6501,11 @@
         <f t="shared" si="7"/>
         <v>94611371</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="3">
         <f t="shared" si="5"/>
         <v>17138323546.541969</v>
       </c>
-      <c r="E87">
+      <c r="E87" s="3">
         <f t="shared" si="8"/>
         <v>125599295013.56747</v>
       </c>
@@ -6513,11 +6522,11 @@
         <f t="shared" si="7"/>
         <v>106196695</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="3">
         <f t="shared" si="5"/>
         <v>19846178666.895599</v>
       </c>
-      <c r="E88">
+      <c r="E88" s="3">
         <f t="shared" si="8"/>
         <v>145445473680.46307</v>
       </c>
@@ -6534,11 +6543,11 @@
         <f t="shared" si="7"/>
         <v>119200772</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="3">
         <f t="shared" si="5"/>
         <v>22981874896.265102</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="3">
         <f t="shared" si="8"/>
         <v>168427348576.72818</v>
       </c>
@@ -6555,11 +6564,11 @@
         <f t="shared" si="7"/>
         <v>133797345</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="3">
         <f t="shared" si="5"/>
         <v>26613011129.874989</v>
       </c>
-      <c r="E90">
+      <c r="E90" s="3">
         <f t="shared" si="8"/>
         <v>195040359706.60318</v>
       </c>
@@ -6576,11 +6585,11 @@
         <f t="shared" si="7"/>
         <v>150181435</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="3">
         <f t="shared" si="5"/>
         <v>30817866888.395233</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="3">
         <f t="shared" si="8"/>
         <v>225858226594.99841</v>
       </c>
@@ -6597,11 +6606,11 @@
         <f t="shared" si="7"/>
         <v>168571944</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="3">
         <f t="shared" si="5"/>
         <v>35687089856.761681</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="3">
         <f t="shared" si="8"/>
         <v>261545316451.7601</v>
       </c>
@@ -6618,11 +6627,11 @@
         <f t="shared" si="7"/>
         <v>189214582</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="3">
         <f t="shared" si="5"/>
         <v>41325650054.13002</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="3">
         <f t="shared" si="8"/>
         <v>302870966505.89014</v>
       </c>
@@ -6639,11 +6648,11 @@
         <f t="shared" si="7"/>
         <v>212385150</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="3">
         <f t="shared" si="5"/>
         <v>47855102762.682556</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="3">
         <f t="shared" si="8"/>
         <v>350726069268.57269</v>
       </c>
@@ -6660,11 +6669,11 @@
         <f t="shared" si="7"/>
         <v>238393222</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="3">
         <f t="shared" si="5"/>
         <v>55416208999.186394</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="3">
         <f t="shared" si="8"/>
         <v>406142278267.75909</v>
       </c>
@@ -6681,11 +6690,11 @@
         <f t="shared" si="7"/>
         <v>267586286</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="3">
         <f t="shared" ref="D96:D159" si="9">D95*1.158</f>
         <v>64171970021.057838</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="3">
         <f t="shared" si="8"/>
         <v>470314248288.81696</v>
       </c>
@@ -6702,11 +6711,11 @@
         <f t="shared" si="7"/>
         <v>300354382</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="3">
         <f t="shared" si="9"/>
         <v>74311141284.384979</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="3">
         <f t="shared" si="8"/>
         <v>544625389573.2019</v>
       </c>
@@ -6723,11 +6732,11 @@
         <f t="shared" si="7"/>
         <v>337135315</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="3">
         <f t="shared" si="9"/>
         <v>86052301607.317795</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="3">
         <f t="shared" si="8"/>
         <v>630677691180.51965</v>
       </c>
@@ -6744,11 +6753,11 @@
         <f t="shared" si="7"/>
         <v>378420505</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="3">
         <f t="shared" si="9"/>
         <v>99648565261.274002</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="3">
         <f t="shared" si="8"/>
         <v>730326256441.7937</v>
       </c>
@@ -6765,11 +6774,11 @@
         <f t="shared" si="7"/>
         <v>424761554</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="3">
         <f t="shared" si="9"/>
         <v>115393038572.55528</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="3">
         <f t="shared" si="8"/>
         <v>845719295014.349</v>
       </c>
@@ -6786,11 +6795,11 @@
         <f t="shared" si="7"/>
         <v>476777611</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="3">
         <f t="shared" si="9"/>
         <v>133625138667.01901</v>
       </c>
-      <c r="E101">
+      <c r="E101" s="3">
         <f t="shared" si="8"/>
         <v>979344433681.36804</v>
       </c>
@@ -6807,11 +6816,11 @@
         <f t="shared" si="7"/>
         <v>535163650</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="3">
         <f t="shared" si="9"/>
         <v>154737910576.40802</v>
       </c>
-      <c r="E102">
+      <c r="E102" s="3">
         <f t="shared" si="8"/>
         <v>1134082344257.7761</v>
       </c>
@@ -6828,11 +6837,11 @@
         <f t="shared" si="7"/>
         <v>600699752</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="3">
         <f t="shared" si="9"/>
         <v>179186500447.48047</v>
       </c>
-      <c r="E103">
+      <c r="E103" s="3">
         <f t="shared" si="8"/>
         <v>1313268844705.2566</v>
       </c>
@@ -6849,11 +6858,11 @@
         <f t="shared" si="7"/>
         <v>674261527</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="3">
         <f t="shared" si="9"/>
         <v>207497967518.18237</v>
       </c>
-      <c r="E104">
+      <c r="E104" s="3">
         <f t="shared" si="8"/>
         <v>1520766812223.439</v>
       </c>
@@ -6870,11 +6879,11 @@
         <f t="shared" si="7"/>
         <v>756831816</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="3">
         <f t="shared" si="9"/>
         <v>240282646386.05518</v>
       </c>
-      <c r="E105">
+      <c r="E105" s="3">
         <f t="shared" si="8"/>
         <v>1761049458609.4941</v>
       </c>
@@ -6891,11 +6900,11 @@
         <f t="shared" si="7"/>
         <v>849513821</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="3">
         <f t="shared" si="9"/>
         <v>278247304515.05188</v>
       </c>
-      <c r="E106">
+      <c r="E106" s="3">
         <f t="shared" si="8"/>
         <v>2039296763124.5459</v>
       </c>
@@ -6912,11 +6921,11 @@
         <f t="shared" si="7"/>
         <v>953545842</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="3">
         <f t="shared" si="9"/>
         <v>322210378628.43005</v>
       </c>
-      <c r="E107">
+      <c r="E107" s="3">
         <f t="shared" si="8"/>
         <v>2361507141752.9761</v>
       </c>
@@ -6933,11 +6942,11 @@
         <f t="shared" si="7"/>
         <v>1070317825</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="3">
         <f t="shared" si="9"/>
         <v>373119618451.72198</v>
       </c>
-      <c r="E108">
+      <c r="E108" s="3">
         <f t="shared" si="8"/>
         <v>2734626760204.6982</v>
       </c>
@@ -6954,11 +6963,11 @@
         <f t="shared" si="7"/>
         <v>1201389933</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="3">
         <f t="shared" si="9"/>
         <v>432072518167.09406</v>
       </c>
-      <c r="E109">
+      <c r="E109" s="3">
         <f t="shared" si="8"/>
         <v>3166699278371.7925</v>
       </c>
@@ -6975,11 +6984,11 @@
         <f t="shared" si="7"/>
         <v>1348513387</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="3">
         <f t="shared" si="9"/>
         <v>500339976037.49487</v>
       </c>
-      <c r="E110">
+      <c r="E110" s="3">
         <f t="shared" si="8"/>
         <v>3667039254409.2871</v>
       </c>
@@ -6996,11 +7005,11 @@
         <f t="shared" si="7"/>
         <v>1513653868</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="3">
         <f t="shared" si="9"/>
         <v>579393692251.41907</v>
       </c>
-      <c r="E111">
+      <c r="E111" s="3">
         <f t="shared" si="8"/>
         <v>4246432946660.7061</v>
       </c>
@@ -7017,11 +7026,11 @@
         <f t="shared" si="7"/>
         <v>1699017779</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="3">
         <f t="shared" si="9"/>
         <v>670937895627.14319</v>
       </c>
-      <c r="E112">
+      <c r="E112" s="3">
         <f t="shared" si="8"/>
         <v>4917370842287.8496</v>
       </c>
@@ -7038,11 +7047,11 @@
         <f t="shared" si="7"/>
         <v>1907081721</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="3">
         <f t="shared" si="9"/>
         <v>776946083136.23181</v>
       </c>
-      <c r="E113">
+      <c r="E113" s="3">
         <f t="shared" si="8"/>
         <v>5694316925424.0811</v>
       </c>
@@ -7059,11 +7068,11 @@
         <f t="shared" si="7"/>
         <v>2140625587</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="3">
         <f t="shared" si="9"/>
         <v>899703564271.75635</v>
       </c>
-      <c r="E114">
+      <c r="E114" s="3">
         <f t="shared" si="8"/>
         <v>6594020489695.8379</v>
       </c>
@@ -7080,11 +7089,11 @@
         <f t="shared" si="7"/>
         <v>2402769701</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="3">
         <f t="shared" si="9"/>
         <v>1041856727426.6937</v>
       </c>
-      <c r="E115">
+      <c r="E115" s="3">
         <f t="shared" si="8"/>
         <v>7635877217122.5313</v>
       </c>
@@ -7101,11 +7110,11 @@
         <f t="shared" si="7"/>
         <v>2697016507</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="3">
         <f t="shared" si="9"/>
         <v>1206470090360.1113</v>
       </c>
-      <c r="E116">
+      <c r="E116" s="3">
         <f t="shared" si="8"/>
         <v>8842347307482.6426</v>
       </c>
@@ -7122,11 +7131,11 @@
         <f t="shared" si="7"/>
         <v>3027297366</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="3">
         <f t="shared" si="9"/>
         <v>1397092364637.0088</v>
       </c>
-      <c r="E117">
+      <c r="E117" s="3">
         <f t="shared" si="8"/>
         <v>10239439672119.652</v>
       </c>
@@ -7143,11 +7152,11 @@
         <f t="shared" si="7"/>
         <v>3398025083</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="3">
         <f t="shared" si="9"/>
         <v>1617832958249.656</v>
       </c>
-      <c r="E118">
+      <c r="E118" s="3">
         <f t="shared" si="8"/>
         <v>11857272630369.309</v>
       </c>
@@ -7164,11 +7173,11 @@
         <f t="shared" si="7"/>
         <v>3814152862</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="3">
         <f t="shared" si="9"/>
         <v>1873450565653.1016</v>
       </c>
-      <c r="E119">
+      <c r="E119" s="3">
         <f t="shared" si="8"/>
         <v>13730723196022.41</v>
       </c>
@@ -7185,11 +7194,11 @@
         <f t="shared" si="7"/>
         <v>4281240488</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="3">
         <f t="shared" si="9"/>
         <v>2169455755026.2915</v>
       </c>
-      <c r="E120">
+      <c r="E120" s="3">
         <f t="shared" si="8"/>
         <v>15900178951048.701</v>
       </c>
@@ -7206,11 +7215,11 @@
         <f t="shared" si="7"/>
         <v>4805528608</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="3">
         <f t="shared" si="9"/>
         <v>2512229764320.4453</v>
       </c>
-      <c r="E121">
+      <c r="E121" s="3">
         <f t="shared" si="8"/>
         <v>18412408715369.148</v>
       </c>
@@ -7227,11 +7236,11 @@
         <f t="shared" si="7"/>
         <v>5394022111</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="3">
         <f t="shared" si="9"/>
         <v>2909162067083.0757</v>
       </c>
-      <c r="E122">
+      <c r="E122" s="3">
         <f t="shared" si="8"/>
         <v>21321570782452.223</v>
       </c>
@@ -7248,11 +7257,11 @@
         <f t="shared" si="7"/>
         <v>6054583720</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="3">
         <f t="shared" si="9"/>
         <v>3368809673682.2012</v>
       </c>
-      <c r="E123">
+      <c r="E123" s="3">
         <f t="shared" si="8"/>
         <v>24690380456134.422</v>
       </c>
@@ -7269,11 +7278,11 @@
         <f t="shared" si="7"/>
         <v>6796039043</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="3">
         <f t="shared" si="9"/>
         <v>3901081602123.9888</v>
       </c>
-      <c r="E124">
+      <c r="E124" s="3">
         <f t="shared" si="8"/>
         <v>28591462058258.41</v>
       </c>
@@ -7290,11 +7299,11 @@
         <f t="shared" si="7"/>
         <v>7628294489</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="3">
         <f t="shared" si="9"/>
         <v>4517452495259.5791</v>
       </c>
-      <c r="E125">
+      <c r="E125" s="3">
         <f t="shared" si="8"/>
         <v>33108914553517.988</v>
       </c>
@@ -7311,11 +7320,11 @@
         <f t="shared" si="7"/>
         <v>8562469628</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="3">
         <f t="shared" si="9"/>
         <v>5231209989510.5918</v>
       </c>
-      <c r="E126">
+      <c r="E126" s="3">
         <f t="shared" si="8"/>
         <v>38340124543028.578</v>
       </c>
@@ -7332,11 +7341,11 @@
         <f t="shared" si="7"/>
         <v>9611045754</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="3">
         <f t="shared" si="9"/>
         <v>6057741167853.2646</v>
       </c>
-      <c r="E127">
+      <c r="E127" s="3">
         <f t="shared" si="8"/>
         <v>44397865710881.844</v>
       </c>
@@ -7353,11 +7362,11 @@
         <f t="shared" si="7"/>
         <v>10788032645</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="3">
         <f t="shared" si="9"/>
         <v>7014864272374.0801</v>
       </c>
-      <c r="E128">
+      <c r="E128" s="3">
         <f t="shared" si="8"/>
         <v>51412729983255.922</v>
       </c>
@@ -7374,11 +7383,11 @@
         <f t="shared" si="7"/>
         <v>12109155747</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="3">
         <f t="shared" si="9"/>
         <v>8123212827409.1846</v>
       </c>
-      <c r="E129">
+      <c r="E129" s="3">
         <f t="shared" si="8"/>
         <v>59535942810665.109</v>
       </c>
@@ -7395,11 +7404,11 @@
         <f t="shared" si="7"/>
         <v>13592066276</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="3">
         <f t="shared" si="9"/>
         <v>9406680454139.8359</v>
       </c>
-      <c r="E130">
+      <c r="E130" s="3">
         <f t="shared" si="8"/>
         <v>68942623264804.945</v>
       </c>
@@ -7416,11 +7425,11 @@
         <f t="shared" si="7"/>
         <v>15256577051</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="3">
         <f t="shared" si="9"/>
         <v>10892935965893.93</v>
       </c>
-      <c r="E131">
+      <c r="E131" s="3">
         <f t="shared" si="8"/>
         <v>79835559230698.875</v>
       </c>
@@ -7437,11 +7446,11 @@
         <f t="shared" ref="C132:C195" si="11">B132+C131</f>
         <v>17124927210</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="3">
         <f t="shared" si="9"/>
         <v>12614019848505.17</v>
       </c>
-      <c r="E132">
+      <c r="E132" s="3">
         <f t="shared" ref="E132:E195" si="12">D132+E131</f>
         <v>92449579079204.047</v>
       </c>
@@ -7458,11 +7467,11 @@
         <f t="shared" si="11"/>
         <v>19222079342</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="3">
         <f t="shared" si="9"/>
         <v>14607034984568.986</v>
       </c>
-      <c r="E133">
+      <c r="E133" s="3">
         <f t="shared" si="12"/>
         <v>107056614063773.03</v>
       </c>
@@ -7479,11 +7488,11 @@
         <f t="shared" si="11"/>
         <v>21576053004</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="3">
         <f t="shared" si="9"/>
         <v>16914946512130.885</v>
       </c>
-      <c r="E134">
+      <c r="E134" s="3">
         <f t="shared" si="12"/>
         <v>123971560575903.92</v>
       </c>
@@ -7500,11 +7509,11 @@
         <f t="shared" si="11"/>
         <v>24218299087</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="3">
         <f t="shared" si="9"/>
         <v>19587508061047.563</v>
       </c>
-      <c r="E135">
+      <c r="E135" s="3">
         <f t="shared" si="12"/>
         <v>143559068636951.5</v>
       </c>
@@ -7521,11 +7530,11 @@
         <f t="shared" si="11"/>
         <v>27184120022</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="3">
         <f t="shared" si="9"/>
         <v>22682334334693.074</v>
       </c>
-      <c r="E136">
+      <c r="E136" s="3">
         <f t="shared" si="12"/>
         <v>166241402971644.56</v>
       </c>
@@ -7542,11 +7551,11 @@
         <f t="shared" si="11"/>
         <v>30513141448</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="3">
         <f t="shared" si="9"/>
         <v>26266143159574.578</v>
       </c>
-      <c r="E137">
+      <c r="E137" s="3">
         <f t="shared" si="12"/>
         <v>192507546131219.13</v>
       </c>
@@ -7563,11 +7572,11 @@
         <f t="shared" si="11"/>
         <v>34249841642</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="3">
         <f t="shared" si="9"/>
         <v>30416193778787.359</v>
       </c>
-      <c r="E138">
+      <c r="E138" s="3">
         <f t="shared" si="12"/>
         <v>222923739910006.5</v>
       </c>
@@ -7584,11 +7593,11 @@
         <f t="shared" si="11"/>
         <v>38444145780</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="3">
         <f t="shared" si="9"/>
         <v>35221952395835.758</v>
       </c>
-      <c r="E139">
+      <c r="E139" s="3">
         <f t="shared" si="12"/>
         <v>258145692305842.25</v>
       </c>
@@ -7605,11 +7614,11 @@
         <f t="shared" si="11"/>
         <v>43152092978</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="3">
         <f t="shared" si="9"/>
         <v>40787020874377.805</v>
       </c>
-      <c r="E140">
+      <c r="E140" s="3">
         <f t="shared" si="12"/>
         <v>298932713180220.06</v>
       </c>
@@ -7626,11 +7635,11 @@
         <f t="shared" si="11"/>
         <v>48436585017</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="3">
         <f t="shared" si="9"/>
         <v>47231370172529.492</v>
       </c>
-      <c r="E141">
+      <c r="E141" s="3">
         <f t="shared" si="12"/>
         <v>346164083352749.56</v>
       </c>
@@ -7647,11 +7656,11 @@
         <f t="shared" si="11"/>
         <v>54368226759</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="3">
         <f t="shared" si="9"/>
         <v>54693926659789.148</v>
       </c>
-      <c r="E142">
+      <c r="E142" s="3">
         <f t="shared" si="12"/>
         <v>400858010012538.69</v>
       </c>
@@ -7668,11 +7677,11 @@
         <f t="shared" si="11"/>
         <v>61026269482</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="3">
         <f t="shared" si="9"/>
         <v>63335567072035.828</v>
       </c>
-      <c r="E143">
+      <c r="E143" s="3">
         <f t="shared" si="12"/>
         <v>464193577084574.5</v>
       </c>
@@ -7689,11 +7698,11 @@
         <f t="shared" si="11"/>
         <v>68499669739</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="3">
         <f t="shared" si="9"/>
         <v>73342586669417.484</v>
       </c>
-      <c r="E144">
+      <c r="E144" s="3">
         <f t="shared" si="12"/>
         <v>537536163753992</v>
       </c>
@@ -7710,11 +7719,11 @@
         <f t="shared" si="11"/>
         <v>76888277883</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="3">
         <f t="shared" si="9"/>
         <v>84930715363185.438</v>
       </c>
-      <c r="E145">
+      <c r="E145" s="3">
         <f t="shared" si="12"/>
         <v>622466879117177.5</v>
       </c>
@@ -7731,11 +7740,11 @@
         <f t="shared" si="11"/>
         <v>86304172146</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="3">
         <f t="shared" si="9"/>
         <v>98349768390568.734</v>
       </c>
-      <c r="E146">
+      <c r="E146" s="3">
         <f t="shared" si="12"/>
         <v>720816647507746.25</v>
       </c>
@@ -7752,11 +7761,11 @@
         <f t="shared" si="11"/>
         <v>96873156090</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="3">
         <f t="shared" si="9"/>
         <v>113889031796278.59</v>
       </c>
-      <c r="E147">
+      <c r="E147" s="3">
         <f t="shared" si="12"/>
         <v>834705679304024.88</v>
       </c>
@@ -7773,11 +7782,11 @@
         <f t="shared" si="11"/>
         <v>108736439440</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="3">
         <f t="shared" si="9"/>
         <v>131883498820090.61</v>
       </c>
-      <c r="E148">
+      <c r="E148" s="3">
         <f t="shared" si="12"/>
         <v>966589178124115.5</v>
       </c>
@@ -7794,11 +7803,11 @@
         <f t="shared" si="11"/>
         <v>122052524751</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="3">
         <f t="shared" si="9"/>
         <v>152721091633664.91</v>
       </c>
-      <c r="E149">
+      <c r="E149" s="3">
         <f t="shared" si="12"/>
         <v>1119310269757780.4</v>
       </c>
@@ -7815,11 +7824,11 @@
         <f t="shared" si="11"/>
         <v>136999325128</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="3">
         <f t="shared" si="9"/>
         <v>176851024111783.94</v>
       </c>
-      <c r="E150">
+      <c r="E150" s="3">
         <f t="shared" si="12"/>
         <v>1296161293869564.3</v>
       </c>
@@ -7836,11 +7845,11 @@
         <f t="shared" si="11"/>
         <v>153776541278</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="3">
         <f t="shared" si="9"/>
         <v>204793485921445.78</v>
       </c>
-      <c r="E151">
+      <c r="E151" s="3">
         <f t="shared" si="12"/>
         <v>1500954779791010</v>
       </c>
@@ -7857,11 +7866,11 @@
         <f t="shared" si="11"/>
         <v>172608329665</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="3">
         <f t="shared" si="9"/>
         <v>237150856697034.19</v>
       </c>
-      <c r="E152">
+      <c r="E152" s="3">
         <f t="shared" si="12"/>
         <v>1738105636488044.3</v>
       </c>
@@ -7878,11 +7887,11 @@
         <f t="shared" si="11"/>
         <v>193746297414</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="3">
         <f t="shared" si="9"/>
         <v>274620692055165.56</v>
       </c>
-      <c r="E153">
+      <c r="E153" s="3">
         <f t="shared" si="12"/>
         <v>2012726328543209.8</v>
       </c>
@@ -7899,11 +7908,11 @@
         <f t="shared" si="11"/>
         <v>217472863973</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="3">
         <f t="shared" si="9"/>
         <v>318010761399881.69</v>
       </c>
-      <c r="E154">
+      <c r="E154" s="3">
         <f t="shared" si="12"/>
         <v>2330737089943091.5</v>
       </c>
@@ -7920,11 +7929,11 @@
         <f t="shared" si="11"/>
         <v>244105034454</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="3">
         <f t="shared" si="9"/>
         <v>368256461701062.94</v>
       </c>
-      <c r="E155">
+      <c r="E155" s="3">
         <f t="shared" si="12"/>
         <v>2698993551644154.5</v>
       </c>
@@ -7941,11 +7950,11 @@
         <f t="shared" si="11"/>
         <v>273998635065</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="3">
         <f t="shared" si="9"/>
         <v>426440982649830.88</v>
       </c>
-      <c r="E156">
+      <c r="E156" s="3">
         <f t="shared" si="12"/>
         <v>3125434534293985.5</v>
       </c>
@@ -7962,11 +7971,11 @@
         <f t="shared" si="11"/>
         <v>307553067221</v>
       </c>
-      <c r="D157">
+      <c r="D157" s="3">
         <f t="shared" si="9"/>
         <v>493818657908504.13</v>
       </c>
-      <c r="E157">
+      <c r="E157" s="3">
         <f t="shared" si="12"/>
         <v>3619253192202489.5</v>
       </c>
@@ -7983,11 +7992,11 @@
         <f t="shared" si="11"/>
         <v>345216643850</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="3">
         <f t="shared" si="9"/>
         <v>571842005858047.75</v>
       </c>
-      <c r="E158">
+      <c r="E158" s="3">
         <f t="shared" si="12"/>
         <v>4191095198060537</v>
       </c>
@@ -8004,11 +8013,11 @@
         <f t="shared" si="11"/>
         <v>387492579202</v>
       </c>
-      <c r="D159">
+      <c r="D159" s="3">
         <f t="shared" si="9"/>
         <v>662193042783619.25</v>
       </c>
-      <c r="E159">
+      <c r="E159" s="3">
         <f t="shared" si="12"/>
         <v>4853288240844156</v>
       </c>
@@ -8025,11 +8034,11 @@
         <f t="shared" si="11"/>
         <v>434945712173</v>
       </c>
-      <c r="D160">
+      <c r="D160" s="3">
         <f t="shared" ref="D160:D201" si="13">D159*1.158</f>
         <v>766819543543431</v>
       </c>
-      <c r="E160">
+      <c r="E160" s="3">
         <f t="shared" si="12"/>
         <v>5620107784387587</v>
       </c>
@@ -8046,11 +8055,11 @@
         <f t="shared" si="11"/>
         <v>488210052987</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="3">
         <f t="shared" si="13"/>
         <v>887977031423293</v>
       </c>
-      <c r="E161">
+      <c r="E161" s="3">
         <f t="shared" si="12"/>
         <v>6508084815810880</v>
       </c>
@@ -8067,11 +8076,11 @@
         <f t="shared" si="11"/>
         <v>547997254061</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="3">
         <f t="shared" si="13"/>
         <v>1028277402388173.3</v>
       </c>
-      <c r="E162">
+      <c r="E162" s="3">
         <f t="shared" si="12"/>
         <v>7536362218199053</v>
       </c>
@@ -8088,11 +8097,11 @@
         <f t="shared" si="11"/>
         <v>615106118223</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="3">
         <f t="shared" si="13"/>
         <v>1190745231965504.5</v>
       </c>
-      <c r="E163">
+      <c r="E163" s="3">
         <f t="shared" si="12"/>
         <v>8727107450164558</v>
       </c>
@@ -8109,11 +8118,11 @@
         <f t="shared" si="11"/>
         <v>690433271331</v>
       </c>
-      <c r="D164">
+      <c r="D164" s="3">
         <f t="shared" si="13"/>
         <v>1378882978616054</v>
       </c>
-      <c r="E164">
+      <c r="E164" s="3">
         <f t="shared" si="12"/>
         <v>1.0105990428780612E+16</v>
       </c>
@@ -8130,11 +8139,11 @@
         <f t="shared" si="11"/>
         <v>774985141883</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="3">
         <f t="shared" si="13"/>
         <v>1596746489237390.5</v>
       </c>
-      <c r="E165">
+      <c r="E165" s="3">
         <f t="shared" si="12"/>
         <v>1.1702736918018002E+16</v>
       </c>
@@ -8151,11 +8160,11 @@
         <f t="shared" si="11"/>
         <v>869891407672</v>
       </c>
-      <c r="D166">
+      <c r="D166" s="3">
         <f t="shared" si="13"/>
         <v>1849032434536898</v>
       </c>
-      <c r="E166">
+      <c r="E166" s="3">
         <f t="shared" si="12"/>
         <v>1.35517693525549E+16</v>
       </c>
@@ -8172,11 +8181,11 @@
         <f t="shared" si="11"/>
         <v>976420089147</v>
       </c>
-      <c r="D167">
+      <c r="D167" s="3">
         <f t="shared" si="13"/>
         <v>2141179559193727.8</v>
       </c>
-      <c r="E167">
+      <c r="E167" s="3">
         <f t="shared" si="12"/>
         <v>1.5692948911748628E+16</v>
       </c>
@@ -8193,11 +8202,11 @@
         <f t="shared" si="11"/>
         <v>1095994491140</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="3">
         <f t="shared" si="13"/>
         <v>2479485929546336.5</v>
       </c>
-      <c r="E168">
+      <c r="E168" s="3">
         <f t="shared" si="12"/>
         <v>1.8172434841294964E+16</v>
       </c>
@@ -8214,11 +8223,11 @@
         <f t="shared" si="11"/>
         <v>1230212219308</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="3">
         <f t="shared" si="13"/>
         <v>2871244706414657.5</v>
       </c>
-      <c r="E169">
+      <c r="E169" s="3">
         <f t="shared" si="12"/>
         <v>2.104367954770962E+16</v>
       </c>
@@ -8235,11 +8244,11 @@
         <f t="shared" si="11"/>
         <v>1380866525367</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="3">
         <f t="shared" si="13"/>
         <v>3324901370028173</v>
       </c>
-      <c r="E170">
+      <c r="E170" s="3">
         <f t="shared" si="12"/>
         <v>2.4368580917737792E+16</v>
       </c>
@@ -8256,11 +8265,11 @@
         <f t="shared" si="11"/>
         <v>1549970266313</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="3">
         <f t="shared" si="13"/>
         <v>3850235786492624</v>
       </c>
-      <c r="E171">
+      <c r="E171" s="3">
         <f t="shared" si="12"/>
         <v>2.8218816704230416E+16</v>
       </c>
@@ -8277,11 +8286,11 @@
         <f t="shared" si="11"/>
         <v>1739782797732</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="3">
         <f t="shared" si="13"/>
         <v>4458573040758458.5</v>
       </c>
-      <c r="E172">
+      <c r="E172" s="3">
         <f t="shared" si="12"/>
         <v>3.2677389744988876E+16</v>
       </c>
@@ -8298,11 +8307,11 @@
         <f t="shared" si="11"/>
         <v>1952840160523</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="3">
         <f t="shared" si="13"/>
         <v>5163027581198295</v>
       </c>
-      <c r="E173">
+      <c r="E173" s="3">
         <f t="shared" si="12"/>
         <v>3.7840417326187168E+16</v>
       </c>
@@ -8319,11 +8328,11 @@
         <f t="shared" si="11"/>
         <v>2191988964349</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="3">
         <f t="shared" si="13"/>
         <v>5978785939027625</v>
       </c>
-      <c r="E174">
+      <c r="E174" s="3">
         <f t="shared" si="12"/>
         <v>4.3819203265214792E+16</v>
       </c>
@@ -8340,11 +8349,11 @@
         <f t="shared" si="11"/>
         <v>2460424420523</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="3">
         <f t="shared" si="13"/>
         <v>6923434117393989</v>
       </c>
-      <c r="E175">
+      <c r="E175" s="3">
         <f t="shared" si="12"/>
         <v>5.0742637382608784E+16</v>
       </c>
@@ -8361,11 +8370,11 @@
         <f t="shared" si="11"/>
         <v>2761733032478</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="3">
         <f t="shared" si="13"/>
         <v>8017336707942239</v>
       </c>
-      <c r="E176">
+      <c r="E176" s="3">
         <f t="shared" si="12"/>
         <v>5.8759974090551024E+16</v>
       </c>
@@ -8382,11 +8391,11 @@
         <f t="shared" si="11"/>
         <v>3099940514206</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="3">
         <f t="shared" si="13"/>
         <v>9284075907797112</v>
       </c>
-      <c r="E177">
+      <c r="E177" s="3">
         <f t="shared" si="12"/>
         <v>6.8044049998348136E+16</v>
       </c>
@@ -8403,11 +8412,11 @@
         <f t="shared" si="11"/>
         <v>3479565576880</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="3">
         <f t="shared" si="13"/>
         <v>1.0750959901229054E+16</v>
       </c>
-      <c r="E178">
+      <c r="E178" s="3">
         <f t="shared" si="12"/>
         <v>7.8795009899577184E+16</v>
       </c>
@@ -8424,11 +8433,11 @@
         <f t="shared" si="11"/>
         <v>3905680302297</v>
       </c>
-      <c r="D179">
+      <c r="D179" s="3">
         <f t="shared" si="13"/>
         <v>1.2449611565623244E+16</v>
       </c>
-      <c r="E179">
+      <c r="E179" s="3">
         <f t="shared" si="12"/>
         <v>9.1244621465200432E+16</v>
       </c>
@@ -8445,11 +8454,11 @@
         <f t="shared" si="11"/>
         <v>4383977909783</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="3">
         <f t="shared" si="13"/>
         <v>1.4416650192991716E+16</v>
       </c>
-      <c r="E180">
+      <c r="E180" s="3">
         <f t="shared" si="12"/>
         <v>1.0566127165819214E+17</v>
       </c>
@@ -8466,11 +8475,11 @@
         <f t="shared" si="11"/>
         <v>4920848821963</v>
       </c>
-      <c r="D181">
+      <c r="D181" s="3">
         <f t="shared" si="13"/>
         <v>1.6694480923484406E+16</v>
       </c>
-      <c r="E181">
+      <c r="E181" s="3">
         <f t="shared" si="12"/>
         <v>1.2235575258167654E+17</v>
       </c>
@@ -8487,11 +8496,11 @@
         <f t="shared" si="11"/>
         <v>5523466045705</v>
       </c>
-      <c r="D182">
+      <c r="D182" s="3">
         <f t="shared" si="13"/>
         <v>1.933220890939494E+16</v>
       </c>
-      <c r="E182">
+      <c r="E182" s="3">
         <f t="shared" si="12"/>
         <v>1.4168796149107149E+17</v>
       </c>
@@ -8508,11 +8517,11 @@
         <f t="shared" si="11"/>
         <v>6199881008992</v>
       </c>
-      <c r="D183">
+      <c r="D183" s="3">
         <f t="shared" si="13"/>
         <v>2.238669791707934E+16</v>
       </c>
-      <c r="E183">
+      <c r="E183" s="3">
         <f t="shared" si="12"/>
         <v>1.6407465940815082E+17</v>
       </c>
@@ -8529,11 +8538,11 @@
         <f t="shared" si="11"/>
         <v>6959131134169</v>
       </c>
-      <c r="D184">
+      <c r="D184" s="3">
         <f t="shared" si="13"/>
         <v>2.5923796187977872E+16</v>
       </c>
-      <c r="E184">
+      <c r="E184" s="3">
         <f t="shared" si="12"/>
         <v>1.899984555961287E+17</v>
       </c>
@@ -8550,11 +8559,11 @@
         <f t="shared" si="11"/>
         <v>7811360584832</v>
       </c>
-      <c r="D185">
+      <c r="D185" s="3">
         <f t="shared" si="13"/>
         <v>3.0019755985678372E+16</v>
       </c>
-      <c r="E185">
+      <c r="E185" s="3">
         <f t="shared" si="12"/>
         <v>2.2001821158180707E+17</v>
       </c>
@@ -8571,11 +8580,11 @@
         <f t="shared" si="11"/>
         <v>8767955799632</v>
       </c>
-      <c r="D186">
+      <c r="D186" s="3">
         <f t="shared" si="13"/>
         <v>3.4762877431415552E+16</v>
       </c>
-      <c r="E186">
+      <c r="E186" s="3">
         <f t="shared" si="12"/>
         <v>2.5478108901322262E+17</v>
       </c>
@@ -8592,11 +8601,11 @@
         <f t="shared" si="11"/>
         <v>9841697623818</v>
       </c>
-      <c r="D187">
+      <c r="D187" s="3">
         <f t="shared" si="13"/>
         <v>4.0255412065579208E+16</v>
       </c>
-      <c r="E187">
+      <c r="E187" s="3">
         <f t="shared" si="12"/>
         <v>2.9503650107880186E+17</v>
       </c>
@@ -8613,11 +8622,11 @@
         <f t="shared" si="11"/>
         <v>11046932071127</v>
       </c>
-      <c r="D188">
+      <c r="D188" s="3">
         <f t="shared" si="13"/>
         <v>4.661576717194072E+16</v>
       </c>
-      <c r="E188">
+      <c r="E188" s="3">
         <f t="shared" si="12"/>
         <v>3.4165226825074259E+17</v>
       </c>
@@ -8634,11 +8643,11 @@
         <f t="shared" si="11"/>
         <v>12399761997525</v>
       </c>
-      <c r="D189">
+      <c r="D189" s="3">
         <f t="shared" si="13"/>
         <v>5.3981058385107352E+16</v>
       </c>
-      <c r="E189">
+      <c r="E189" s="3">
         <f t="shared" si="12"/>
         <v>3.9563332663584992E+17</v>
       </c>
@@ -8655,11 +8664,11 @@
         <f t="shared" si="11"/>
         <v>13918262247702</v>
       </c>
-      <c r="D190">
+      <c r="D190" s="3">
         <f t="shared" si="13"/>
         <v>6.2510065609954312E+16</v>
       </c>
-      <c r="E190">
+      <c r="E190" s="3">
         <f t="shared" si="12"/>
         <v>4.5814339224580422E+17</v>
       </c>
@@ -8676,11 +8685,11 @@
         <f t="shared" si="11"/>
         <v>15622721148851</v>
       </c>
-      <c r="D191">
+      <c r="D191" s="3">
         <f t="shared" si="13"/>
         <v>7.2386655976327088E+16</v>
       </c>
-      <c r="E191">
+      <c r="E191" s="3">
         <f t="shared" si="12"/>
         <v>5.3053004822213133E+17</v>
       </c>
@@ -8697,11 +8706,11 @@
         <f t="shared" si="11"/>
         <v>17535911578272</v>
       </c>
-      <c r="D192">
+      <c r="D192" s="3">
         <f t="shared" si="13"/>
         <v>8.3823747620586768E+16</v>
       </c>
-      <c r="E192">
+      <c r="E192" s="3">
         <f t="shared" si="12"/>
         <v>6.1435379584271808E+17</v>
       </c>
@@ -8718,11 +8727,11 @@
         <f t="shared" si="11"/>
         <v>19683395226464</v>
       </c>
-      <c r="D193">
+      <c r="D193" s="3">
         <f t="shared" si="13"/>
         <v>9.7067899744639472E+16</v>
       </c>
-      <c r="E193">
+      <c r="E193" s="3">
         <f t="shared" si="12"/>
         <v>7.1142169558735757E+17</v>
       </c>
@@ -8739,11 +8748,11 @@
         <f t="shared" si="11"/>
         <v>22093864120901</v>
       </c>
-      <c r="D194">
+      <c r="D194" s="3">
         <f t="shared" si="13"/>
         <v>1.124046279042925E+17</v>
       </c>
-      <c r="E194">
+      <c r="E194" s="3">
         <f t="shared" si="12"/>
         <v>8.2382632349165005E+17</v>
       </c>
@@ -8760,11 +8769,11 @@
         <f t="shared" si="11"/>
         <v>24799523973515</v>
       </c>
-      <c r="D195">
+      <c r="D195" s="3">
         <f t="shared" si="13"/>
         <v>1.301645591131707E+17</v>
       </c>
-      <c r="E195">
+      <c r="E195" s="3">
         <f t="shared" si="12"/>
         <v>9.5399088260482074E+17</v>
       </c>
@@ -8781,11 +8790,11 @@
         <f t="shared" ref="C196:C201" si="15">B196+C195</f>
         <v>27836524473686</v>
       </c>
-      <c r="D196">
+      <c r="D196" s="3">
         <f t="shared" si="13"/>
         <v>1.5073055945305168E+17</v>
       </c>
-      <c r="E196">
+      <c r="E196" s="3">
         <f t="shared" ref="E196:E201" si="16">D196+E195</f>
         <v>1.1047214420578724E+18</v>
       </c>
@@ -8802,11 +8811,11 @@
         <f t="shared" si="15"/>
         <v>31245442275801</v>
       </c>
-      <c r="D197">
+      <c r="D197" s="3">
         <f t="shared" si="13"/>
         <v>1.7454598784663382E+17</v>
       </c>
-      <c r="E197">
+      <c r="E197" s="3">
         <f t="shared" si="16"/>
         <v>1.2792674299045061E+18</v>
       </c>
@@ -8823,11 +8832,11 @@
         <f t="shared" si="15"/>
         <v>35071823134459</v>
       </c>
-      <c r="D198">
+      <c r="D198" s="3">
         <f t="shared" si="13"/>
         <v>2.0212425392640195E+17</v>
       </c>
-      <c r="E198">
+      <c r="E198" s="3">
         <f t="shared" si="16"/>
         <v>1.4813916838309082E+18</v>
       </c>
@@ -8844,11 +8853,11 @@
         <f t="shared" si="15"/>
         <v>39366790430657</v>
       </c>
-      <c r="D199">
+      <c r="D199" s="3">
         <f t="shared" si="13"/>
         <v>2.3405988604677344E+17</v>
       </c>
-      <c r="E199">
+      <c r="E199" s="3">
         <f t="shared" si="16"/>
         <v>1.7154515698776817E+18</v>
       </c>
@@ -8865,11 +8874,11 @@
         <f t="shared" si="15"/>
         <v>44187728219345</v>
       </c>
-      <c r="D200">
+      <c r="D200" s="3">
         <f t="shared" si="13"/>
         <v>2.7104134804216362E+17</v>
       </c>
-      <c r="E200">
+      <c r="E200" s="3">
         <f t="shared" si="16"/>
         <v>1.9864929179198454E+18</v>
       </c>
@@ -8886,11 +8895,11 @@
         <f t="shared" si="15"/>
         <v>49599047924385</v>
       </c>
-      <c r="D201">
+      <c r="D201" s="3">
         <f t="shared" si="13"/>
         <v>3.1386588103282547E+17</v>
       </c>
-      <c r="E201">
+      <c r="E201" s="3">
         <f t="shared" si="16"/>
         <v>2.3003587989526707E+18</v>
       </c>
@@ -8906,7 +8915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated fontawesome. Modified create object functionality to display on table isntead of in modals.
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
-    <sheet name="Monsters" sheetId="2" r:id="rId2"/>
-    <sheet name="d2 mean mlvl" sheetId="6" r:id="rId3"/>
+    <sheet name="d2 mean mlvl" sheetId="6" r:id="rId2"/>
+    <sheet name="Monsters" sheetId="2" r:id="rId3"/>
     <sheet name="Damage Types" sheetId="3" r:id="rId4"/>
     <sheet name="Attack Type" sheetId="4" r:id="rId5"/>
+    <sheet name="Enemy_Modifiers" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>level</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
   </si>
   <si>
     <t>Experience</t>
@@ -175,6 +179,69 @@
   </si>
   <si>
     <t>hell</t>
+  </si>
+  <si>
+    <t>Modifier</t>
+  </si>
+  <si>
+    <t>Chilled</t>
+  </si>
+  <si>
+    <t>Frozen</t>
+  </si>
+  <si>
+    <t>Flaming</t>
+  </si>
+  <si>
+    <t>Burning</t>
+  </si>
+  <si>
+    <t>elemental-Ice</t>
+  </si>
+  <si>
+    <t>elemental-fire</t>
+  </si>
+  <si>
+    <t>Modifier_Type</t>
+  </si>
+  <si>
+    <t>Additive</t>
+  </si>
+  <si>
+    <t>Multiplicative</t>
+  </si>
+  <si>
+    <t>damage_type</t>
+  </si>
+  <si>
+    <t>Rotten</t>
+  </si>
+  <si>
+    <t>Necrotic</t>
+  </si>
+  <si>
+    <t>elemental-poison</t>
+  </si>
+  <si>
+    <t>Lucrative</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>chanceOfItem</t>
+  </si>
+  <si>
+    <t>Rich</t>
+  </si>
+  <si>
+    <t>chanceOfGold</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Rarity (chance of effect occurring)</t>
   </si>
 </sst>
 </file>
@@ -4679,10 +4746,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
   <dimension ref="A1:R201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,13 +4766,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -5064,7 +5134,7 @@
         <v>1616947.9970703125</v>
       </c>
       <c r="H19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
@@ -5088,7 +5158,7 @@
         <v>2046959.7463378906</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R20" t="s">
         <v>1</v>
@@ -5115,7 +5185,7 @@
         <v>2584474.4329223633</v>
       </c>
       <c r="H21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="R21" t="s">
         <v>3</v>
@@ -5142,7 +5212,7 @@
         <v>3256367.7911529541</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
@@ -8913,10 +8983,112 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3">
+        <v>46</v>
+      </c>
+      <c r="D3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>52</v>
+      </c>
+      <c r="D4">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+      <c r="C5">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6">
+        <v>33</v>
+      </c>
+      <c r="C6">
+        <v>63</v>
+      </c>
+      <c r="D6">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="O1" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8933,84 +9105,84 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -9019,104 +9191,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>39</v>
-      </c>
-      <c r="D2">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3">
-        <v>46</v>
-      </c>
-      <c r="D3">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4">
-        <v>23</v>
-      </c>
-      <c r="C4">
-        <v>52</v>
-      </c>
-      <c r="D4">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5">
-        <v>27</v>
-      </c>
-      <c r="C5">
-        <v>57</v>
-      </c>
-      <c r="D5">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6">
-        <v>33</v>
-      </c>
-      <c r="C6">
-        <v>63</v>
-      </c>
-      <c r="D6">
-        <v>83</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9132,80 +9211,80 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
         <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -9215,6 +9294,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9233,12 +9315,219 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3">
+        <v>1.5</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" t="s">
+        <v>56</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5">
+        <v>1.5</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7">
+        <v>1.5</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8">
+        <v>1.5</v>
+      </c>
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated spreadsheet with notes around item join tables`
</commit_message>
<xml_diff>
--- a/Experience curve + formula.xlsx
+++ b/Experience curve + formula.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\request\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\gamerequest\request\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Experience" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,10 @@
     <sheet name="Damage Types" sheetId="3" r:id="rId4"/>
     <sheet name="Attack Type" sheetId="4" r:id="rId5"/>
     <sheet name="Enemy_Modifiers" sheetId="7" r:id="rId6"/>
+    <sheet name="unique-set-items" sheetId="8" r:id="rId7"/>
+    <sheet name="item-types" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
   <si>
     <t>level</t>
   </si>
@@ -243,11 +245,44 @@
   <si>
     <t>Rarity (chance of effect occurring)</t>
   </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>weapon_type_id</t>
+  </si>
+  <si>
+    <t>item_rarity_id</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Weapon</t>
+  </si>
+  <si>
+    <t>weapon</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>consumable</t>
+  </si>
+  <si>
+    <t>potion</t>
+  </si>
+  <si>
+    <t>scroll</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -309,7 +344,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -710,7 +745,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-DB56-4269-896A-90686F91B9B8}"/>
             </c:ext>
@@ -725,11 +760,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1032963888"/>
-        <c:axId val="983738880"/>
+        <c:axId val="1039528736"/>
+        <c:axId val="1225803472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1032963888"/>
+        <c:axId val="1039528736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +806,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="983738880"/>
+        <c:crossAx val="1225803472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -779,7 +814,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="983738880"/>
+        <c:axId val="1225803472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +865,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1032963888"/>
+        <c:crossAx val="1039528736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -880,7 +915,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1579,7 +1614,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-99A5-4BF7-8783-66F2421F2B15}"/>
             </c:ext>
@@ -1594,11 +1629,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="914611168"/>
-        <c:axId val="792954032"/>
+        <c:axId val="1225806736"/>
+        <c:axId val="1225810544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="914611168"/>
+        <c:axId val="1225806736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1640,7 +1675,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="792954032"/>
+        <c:crossAx val="1225810544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1648,7 +1683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="792954032"/>
+        <c:axId val="1225810544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="914611168"/>
+        <c:crossAx val="1225806736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1749,7 +1784,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2230,7 +2265,7 @@
                   <c:v>16914946512130.885</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>19587508061047.563</c:v>
+                  <c:v>19587508061047.562</c:v>
                 </c:pt>
                 <c:pt idx="134">
                   <c:v>22682334334693.074</c:v>
@@ -2260,7 +2295,7 @@
                   <c:v>73342586669417.484</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>84930715363185.438</c:v>
+                  <c:v>84930715363185.437</c:v>
                 </c:pt>
                 <c:pt idx="144">
                   <c:v>98349768390568.734</c:v>
@@ -2293,10 +2328,10 @@
                   <c:v>368256461701062.94</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>426440982649830.88</c:v>
+                  <c:v>426440982649830.87</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>493818657908504.13</c:v>
+                  <c:v>493818657908504.12</c:v>
                 </c:pt>
                 <c:pt idx="156">
                   <c:v>571842005858047.75</c:v>
@@ -2311,7 +2346,7 @@
                   <c:v>887977031423293</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>1028277402388173.3</c:v>
+                  <c:v>1028277402388173.2</c:v>
                 </c:pt>
                 <c:pt idx="161">
                   <c:v>1190745231965504.5</c:v>
@@ -2326,7 +2361,7 @@
                   <c:v>1849032434536898</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>2141179559193727.8</c:v>
+                  <c:v>2141179559193727.7</c:v>
                 </c:pt>
                 <c:pt idx="166">
                   <c:v>2479485929546336.5</c:v>
@@ -2434,7 +2469,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-C4E4-44CA-A175-CF2A08375C1D}"/>
             </c:ext>
@@ -2449,11 +2484,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="220683040"/>
-        <c:axId val="354917984"/>
+        <c:axId val="1225804016"/>
+        <c:axId val="1225811632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="220683040"/>
+        <c:axId val="1225804016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2495,7 +2530,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354917984"/>
+        <c:crossAx val="1225811632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2503,7 +2538,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="354917984"/>
+        <c:axId val="1225811632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2554,7 +2589,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="220683040"/>
+        <c:crossAx val="1225804016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4291,7 +4326,7 @@
         <xdr:cNvPr id="7" name="Picture 6" descr="http://rsdo.net/rsdonline/guides/exp_formula.gif">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30700BDC-240A-428C-A163-B494300D742C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{30700BDC-240A-428C-A163-B494300D742C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4352,7 +4387,7 @@
         <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94D98B5-3D93-4335-93C8-60FCD0092ABC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E94D98B5-3D93-4335-93C8-60FCD0092ABC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4390,7 +4425,7 @@
         <xdr:cNvPr id="11" name="Chart 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49164D1C-84E7-4F1F-85CF-43FD42690072}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{49164D1C-84E7-4F1F-85CF-43FD42690072}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4428,7 +4463,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{677474AB-896D-47F5-A206-B4D22258D6EC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{677474AB-896D-47F5-A206-B4D22258D6EC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4755,13 +4790,13 @@
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.1328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4778,7 +4813,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4792,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4811,7 +4846,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4830,7 +4865,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4849,7 +4884,7 @@
         <v>5750</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4868,7 +4903,7 @@
         <v>13625</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4887,7 +4922,7 @@
         <v>27800</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4907,7 +4942,7 @@
         <v>50480</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4927,7 +4962,7 @@
         <v>83366</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4947,7 +4982,7 @@
         <v>127762</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4967,7 +5002,7 @@
         <v>185477</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -4987,7 +5022,7 @@
         <v>257621</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5008,7 +5043,7 @@
         <v>347801</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5029,7 +5064,7 @@
         <v>460526</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5050,7 +5085,7 @@
         <v>601432.25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5071,7 +5106,7 @@
         <v>777565.0625</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5092,7 +5127,7 @@
         <v>997731.078125</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5113,7 +5148,7 @@
         <v>1272938.59765625</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5137,7 +5172,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5164,7 +5199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5191,7 +5226,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5215,7 +5250,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5236,7 +5271,7 @@
         <v>4096234.4889411926</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5257,7 +5292,7 @@
         <v>5146067.8611764908</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5278,7 +5313,7 @@
         <v>6458359.5764706135</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5299,7 +5334,7 @@
         <v>8098724.2205882668</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5320,7 +5355,7 @@
         <v>10149180.025735334</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -5341,7 +5376,7 @@
         <v>12712249.782169167</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -5362,7 +5397,7 @@
         <v>15916086.977711458</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -5383,7 +5418,7 @@
         <v>19920883.472139321</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -5404,7 +5439,7 @@
         <v>24558437.812686786</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -5425,7 +5460,7 @@
         <v>29928725.739040751</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -5446,7 +5481,7 @@
         <v>36147519.157758646</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -5467,7 +5502,7 @@
         <v>43348881.936633967</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5488,7 +5523,7 @@
         <v>51688060.034571588</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -5509,7 +5544,7 @@
         <v>61344828.271983348</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5530,7 +5565,7 @@
         <v>72527365.89090617</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5551,7 +5586,7 @@
         <v>85476744.453618795</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5572,7 +5607,7 @@
         <v>100472124.82924001</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5593,7 +5628,7 @@
         <v>117836775.30420938</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5614,7 +5649,7 @@
         <v>137945040.5542239</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5635,7 +5670,7 @@
         <v>161230411.71374071</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5656,7 +5691,7 @@
         <v>188194871.51646119</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5677,7 +5712,7 @@
         <v>219419715.9680115</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5698,7 +5733,7 @@
         <v>255578085.84290677</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5719,7 +5754,7 @@
         <v>297449478.15803546</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5740,7 +5775,7 @@
         <v>345936550.45895451</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5761,7 +5796,7 @@
         <v>402084580.18341875</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5782,7 +5817,7 @@
         <v>467103998.60434836</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5803,7 +5838,7 @@
         <v>542396485.13578486</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5824,7 +5859,7 @@
         <v>629585184.53918827</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5845,7 +5880,7 @@
         <v>730549698.44832945</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5866,7 +5901,7 @@
         <v>847466605.55511487</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5887,7 +5922,7 @@
         <v>982856383.98477244</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5908,7 +5943,7 @@
         <v>1139637747.4063158</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5929,7 +5964,7 @@
         <v>1321190566.2484632</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -5950,7 +5985,7 @@
         <v>1531428730.4676697</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -5971,7 +6006,7 @@
         <v>1774884524.6335108</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -5992,7 +6027,7 @@
         <v>2056806334.2775548</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6013,7 +6048,7 @@
         <v>2383271789.8453579</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6034,7 +6069,7 @@
         <v>2761318787.3928738</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6055,7 +6090,7 @@
         <v>3199097210.552897</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6076,7 +6111,7 @@
         <v>3706044624.5722036</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6097,7 +6132,7 @@
         <v>4293089730.0065608</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6118,7 +6153,7 @@
         <v>4972887962.0995464</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6139,7 +6174,7 @@
         <v>5760094314.863224</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6160,7 +6195,7 @@
         <v>6671679271.3635626</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6181,7 +6216,7 @@
         <v>7727294650.9909544</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6202,7 +6237,7 @@
         <v>8949697260.599474</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6223,7 +6258,7 @@
         <v>10365239482.52614</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6244,7 +6279,7 @@
         <v>12004437375.51722</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6265,7 +6300,7 @@
         <v>13902628535.600889</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6286,7 +6321,7 @@
         <v>16100733898.977777</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6307,7 +6342,7 @@
         <v>18646139909.768215</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6328,7 +6363,7 @@
         <v>21593720070.263542</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -6349,7 +6384,7 @@
         <v>25007017896.117126</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -6370,7 +6405,7 @@
         <v>28959616778.455578</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -6391,7 +6426,7 @@
         <v>33536726284.203506</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -6412,7 +6447,7 @@
         <v>38837019091.859604</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -6433,7 +6468,7 @@
         <v>44974758163.125366</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -6454,7 +6489,7 @@
         <v>52082260007.651123</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -6475,7 +6510,7 @@
         <v>60312747143.611946</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -6496,7 +6531,7 @@
         <v>69843651247.054581</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -6517,7 +6552,7 @@
         <v>80880438198.841141</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -6538,7 +6573,7 @@
         <v>93661037489.009979</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -6559,7 +6594,7 @@
         <v>108460971467.0255</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -6580,7 +6615,7 @@
         <v>125599295013.56747</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -6601,7 +6636,7 @@
         <v>145445473680.46307</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -6622,7 +6657,7 @@
         <v>168427348576.72818</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -6643,7 +6678,7 @@
         <v>195040359706.60318</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -6664,7 +6699,7 @@
         <v>225858226594.99841</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -6685,7 +6720,7 @@
         <v>261545316451.7601</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -6706,7 +6741,7 @@
         <v>302870966505.89014</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -6727,7 +6762,7 @@
         <v>350726069268.57269</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -6748,7 +6783,7 @@
         <v>406142278267.75909</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -6769,7 +6804,7 @@
         <v>470314248288.81696</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -6790,7 +6825,7 @@
         <v>544625389573.2019</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -6811,7 +6846,7 @@
         <v>630677691180.51965</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -6832,7 +6867,7 @@
         <v>730326256441.7937</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -6853,7 +6888,7 @@
         <v>845719295014.349</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -6874,7 +6909,7 @@
         <v>979344433681.36804</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -6895,7 +6930,7 @@
         <v>1134082344257.7761</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -6916,7 +6951,7 @@
         <v>1313268844705.2566</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -6937,7 +6972,7 @@
         <v>1520766812223.439</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -6958,7 +6993,7 @@
         <v>1761049458609.4941</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -6979,7 +7014,7 @@
         <v>2039296763124.5459</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -7000,7 +7035,7 @@
         <v>2361507141752.9761</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -7021,7 +7056,7 @@
         <v>2734626760204.6982</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -7042,7 +7077,7 @@
         <v>3166699278371.7925</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -7063,7 +7098,7 @@
         <v>3667039254409.2871</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -7084,7 +7119,7 @@
         <v>4246432946660.7061</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -7105,7 +7140,7 @@
         <v>4917370842287.8496</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -7126,7 +7161,7 @@
         <v>5694316925424.0811</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -7147,7 +7182,7 @@
         <v>6594020489695.8379</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>114</v>
       </c>
@@ -7165,10 +7200,10 @@
       </c>
       <c r="E115" s="3">
         <f t="shared" si="8"/>
-        <v>7635877217122.5313</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7635877217122.5312</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -7189,7 +7224,7 @@
         <v>8842347307482.6426</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -7210,7 +7245,7 @@
         <v>10239439672119.652</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -7231,7 +7266,7 @@
         <v>11857272630369.309</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -7252,7 +7287,7 @@
         <v>13730723196022.41</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -7273,7 +7308,7 @@
         <v>15900178951048.701</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -7294,7 +7329,7 @@
         <v>18412408715369.148</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -7315,7 +7350,7 @@
         <v>21321570782452.223</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -7336,7 +7371,7 @@
         <v>24690380456134.422</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -7357,7 +7392,7 @@
         <v>28591462058258.41</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -7378,7 +7413,7 @@
         <v>33108914553517.988</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -7399,7 +7434,7 @@
         <v>38340124543028.578</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -7420,7 +7455,7 @@
         <v>44397865710881.844</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -7441,7 +7476,7 @@
         <v>51412729983255.922</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -7462,7 +7497,7 @@
         <v>59535942810665.109</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -7483,7 +7518,7 @@
         <v>68942623264804.945</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>130</v>
       </c>
@@ -7504,7 +7539,7 @@
         <v>79835559230698.875</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -7525,7 +7560,7 @@
         <v>92449579079204.047</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -7546,7 +7581,7 @@
         <v>107056614063773.03</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -7567,7 +7602,7 @@
         <v>123971560575903.92</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -7581,14 +7616,14 @@
       </c>
       <c r="D135" s="3">
         <f t="shared" si="9"/>
-        <v>19587508061047.563</v>
+        <v>19587508061047.562</v>
       </c>
       <c r="E135" s="3">
         <f t="shared" si="12"/>
         <v>143559068636951.5</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -7609,7 +7644,7 @@
         <v>166241402971644.56</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -7627,10 +7662,10 @@
       </c>
       <c r="E137" s="3">
         <f t="shared" si="12"/>
-        <v>192507546131219.13</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>192507546131219.12</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -7651,7 +7686,7 @@
         <v>222923739910006.5</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -7672,7 +7707,7 @@
         <v>258145692305842.25</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -7693,7 +7728,7 @@
         <v>298932713180220.06</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -7714,7 +7749,7 @@
         <v>346164083352749.56</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -7735,7 +7770,7 @@
         <v>400858010012538.69</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -7756,7 +7791,7 @@
         <v>464193577084574.5</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -7777,7 +7812,7 @@
         <v>537536163753992</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -7791,14 +7826,14 @@
       </c>
       <c r="D145" s="3">
         <f t="shared" si="9"/>
-        <v>84930715363185.438</v>
+        <v>84930715363185.437</v>
       </c>
       <c r="E145" s="3">
         <f t="shared" si="12"/>
         <v>622466879117177.5</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -7819,7 +7854,7 @@
         <v>720816647507746.25</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -7837,10 +7872,10 @@
       </c>
       <c r="E147" s="3">
         <f t="shared" si="12"/>
-        <v>834705679304024.88</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+        <v>834705679304024.87</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -7861,7 +7896,7 @@
         <v>966589178124115.5</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -7882,7 +7917,7 @@
         <v>1119310269757780.4</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -7900,10 +7935,10 @@
       </c>
       <c r="E150" s="3">
         <f t="shared" si="12"/>
-        <v>1296161293869564.3</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1296161293869564.2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -7924,7 +7959,7 @@
         <v>1500954779791010</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -7942,10 +7977,10 @@
       </c>
       <c r="E152" s="3">
         <f t="shared" si="12"/>
-        <v>1738105636488044.3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1738105636488044.2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -7963,10 +7998,10 @@
       </c>
       <c r="E153" s="3">
         <f t="shared" si="12"/>
-        <v>2012726328543209.8</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2012726328543209.7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -7987,7 +8022,7 @@
         <v>2330737089943091.5</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -8008,7 +8043,7 @@
         <v>2698993551644154.5</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -8022,14 +8057,14 @@
       </c>
       <c r="D156" s="3">
         <f t="shared" si="9"/>
-        <v>426440982649830.88</v>
+        <v>426440982649830.87</v>
       </c>
       <c r="E156" s="3">
         <f t="shared" si="12"/>
         <v>3125434534293985.5</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -8043,14 +8078,14 @@
       </c>
       <c r="D157" s="3">
         <f t="shared" si="9"/>
-        <v>493818657908504.13</v>
+        <v>493818657908504.12</v>
       </c>
       <c r="E157" s="3">
         <f t="shared" si="12"/>
         <v>3619253192202489.5</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -8071,7 +8106,7 @@
         <v>4191095198060537</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -8092,7 +8127,7 @@
         <v>4853288240844156</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -8113,7 +8148,7 @@
         <v>5620107784387587</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -8134,7 +8169,7 @@
         <v>6508084815810880</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -8148,14 +8183,14 @@
       </c>
       <c r="D162" s="3">
         <f t="shared" si="13"/>
-        <v>1028277402388173.3</v>
+        <v>1028277402388173.2</v>
       </c>
       <c r="E162" s="3">
         <f t="shared" si="12"/>
         <v>7536362218199053</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -8176,7 +8211,7 @@
         <v>8727107450164558</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -8197,7 +8232,7 @@
         <v>1.0105990428780612E+16</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -8218,7 +8253,7 @@
         <v>1.1702736918018002E+16</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -8239,7 +8274,7 @@
         <v>1.35517693525549E+16</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -8253,14 +8288,14 @@
       </c>
       <c r="D167" s="3">
         <f t="shared" si="13"/>
-        <v>2141179559193727.8</v>
+        <v>2141179559193727.7</v>
       </c>
       <c r="E167" s="3">
         <f t="shared" si="12"/>
         <v>1.5692948911748628E+16</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -8281,7 +8316,7 @@
         <v>1.8172434841294964E+16</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -8302,7 +8337,7 @@
         <v>2.104367954770962E+16</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -8323,7 +8358,7 @@
         <v>2.4368580917737792E+16</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -8344,7 +8379,7 @@
         <v>2.8218816704230416E+16</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -8365,7 +8400,7 @@
         <v>3.2677389744988876E+16</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -8386,7 +8421,7 @@
         <v>3.7840417326187168E+16</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -8407,7 +8442,7 @@
         <v>4.3819203265214792E+16</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -8428,7 +8463,7 @@
         <v>5.0742637382608784E+16</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -8449,7 +8484,7 @@
         <v>5.8759974090551024E+16</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -8470,7 +8505,7 @@
         <v>6.8044049998348136E+16</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -8491,7 +8526,7 @@
         <v>7.8795009899577184E+16</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>178</v>
       </c>
@@ -8512,7 +8547,7 @@
         <v>9.1244621465200432E+16</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -8533,7 +8568,7 @@
         <v>1.0566127165819214E+17</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -8554,7 +8589,7 @@
         <v>1.2235575258167654E+17</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -8575,7 +8610,7 @@
         <v>1.4168796149107149E+17</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -8596,7 +8631,7 @@
         <v>1.6407465940815082E+17</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -8617,7 +8652,7 @@
         <v>1.899984555961287E+17</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -8638,7 +8673,7 @@
         <v>2.2001821158180707E+17</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -8659,7 +8694,7 @@
         <v>2.5478108901322262E+17</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -8680,7 +8715,7 @@
         <v>2.9503650107880186E+17</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -8701,7 +8736,7 @@
         <v>3.4165226825074259E+17</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -8722,7 +8757,7 @@
         <v>3.9563332663584992E+17</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -8743,7 +8778,7 @@
         <v>4.5814339224580422E+17</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -8764,7 +8799,7 @@
         <v>5.3053004822213133E+17</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -8785,7 +8820,7 @@
         <v>6.1435379584271808E+17</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -8806,7 +8841,7 @@
         <v>7.1142169558735757E+17</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -8827,7 +8862,7 @@
         <v>8.2382632349165005E+17</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -8848,7 +8883,7 @@
         <v>9.5399088260482074E+17</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -8869,7 +8904,7 @@
         <v>1.1047214420578724E+18</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -8890,7 +8925,7 @@
         <v>1.2792674299045061E+18</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -8911,7 +8946,7 @@
         <v>1.4813916838309082E+18</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -8932,7 +8967,7 @@
         <v>1.7154515698776817E+18</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -8953,7 +8988,7 @@
         <v>1.9864929179198454E+18</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -8992,9 +9027,9 @@
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>47</v>
       </c>
@@ -9005,7 +9040,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -9019,7 +9054,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -9033,7 +9068,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -9047,7 +9082,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -9061,7 +9096,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>46</v>
       </c>
@@ -9091,13 +9126,13 @@
       <selection activeCell="O1" sqref="A1:O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="6" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="3" max="6" width="15.3984375" customWidth="1"/>
+    <col min="10" max="10" width="24.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -9144,7 +9179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="71.25" x14ac:dyDescent="0.45">
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
@@ -9202,14 +9237,14 @@
       <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -9223,7 +9258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>13</v>
       </c>
@@ -9231,7 +9266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -9239,7 +9274,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -9247,7 +9282,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -9255,7 +9290,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -9263,7 +9298,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -9271,7 +9306,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -9279,7 +9314,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -9303,9 +9338,9 @@
       <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -9313,12 +9348,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>14</v>
       </c>
@@ -9335,19 +9370,19 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.1328125" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -9370,7 +9405,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>51</v>
       </c>
@@ -9390,7 +9425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>52</v>
       </c>
@@ -9410,7 +9445,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>53</v>
       </c>
@@ -9430,7 +9465,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>54</v>
       </c>
@@ -9450,7 +9485,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>61</v>
       </c>
@@ -9470,7 +9505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>62</v>
       </c>
@@ -9490,7 +9525,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>64</v>
       </c>
@@ -9510,7 +9545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>67</v>
       </c>
@@ -9528,6 +9563,101 @@
       </c>
       <c r="G9">
         <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="9.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>